<commit_message>
Add IFERROR protection to Premier pricing.
Do this because it's plausible for the denominator to fall to zero.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\PHI\0273NYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -1005,20 +1005,20 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
     <col min="3" max="3" width="18" style="70" customWidth="1"/>
-    <col min="4" max="8" width="18.7109375" customWidth="1"/>
+    <col min="4" max="8" width="18.7265625" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" s="60" t="s">
         <v>84</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>43101</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="72" t="s">
         <v>98</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="73"/>
       <c r="C3" s="78"/>
       <c r="D3" s="13" t="s">
@@ -1053,7 +1053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="74" t="s">
         <v>6</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="74" t="s">
         <v>7</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="74" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1107,7 @@
       <c r="G6" s="56"/>
       <c r="H6" s="57"/>
     </row>
-    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="74" t="s">
         <v>5</v>
       </c>
@@ -1123,7 +1123,7 @@
       <c r="G7" s="56"/>
       <c r="H7" s="57"/>
     </row>
-    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="74" t="s">
         <v>9</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="G8" s="56"/>
       <c r="H8" s="57"/>
     </row>
-    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="74" t="s">
         <v>10</v>
       </c>
@@ -1155,7 +1155,7 @@
       <c r="G9" s="56"/>
       <c r="H9" s="57"/>
     </row>
-    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="74" t="s">
         <v>11</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="G10" s="56"/>
       <c r="H10" s="57"/>
     </row>
-    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="74" t="s">
         <v>34</v>
       </c>
@@ -1187,7 +1187,7 @@
       <c r="G11" s="56"/>
       <c r="H11" s="57"/>
     </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="74" t="s">
         <v>12</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="G12" s="56"/>
       <c r="H12" s="57"/>
     </row>
-    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="74" t="s">
         <v>13</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="G13" s="56"/>
       <c r="H13" s="57"/>
     </row>
-    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="74" t="s">
         <v>14</v>
       </c>
@@ -1235,7 +1235,7 @@
       <c r="G14" s="56"/>
       <c r="H14" s="57"/>
     </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="74" t="s">
         <v>15</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="G15" s="56"/>
       <c r="H15" s="57"/>
     </row>
-    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="74" t="s">
         <v>16</v>
       </c>
@@ -1267,7 +1267,7 @@
       <c r="G16" s="56"/>
       <c r="H16" s="57"/>
     </row>
-    <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="74" t="s">
         <v>17</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="G17" s="56"/>
       <c r="H17" s="57"/>
     </row>
-    <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="74" t="s">
         <v>18</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="G18" s="56"/>
       <c r="H18" s="57"/>
     </row>
-    <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="74" t="s">
         <v>19</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="G19" s="56"/>
       <c r="H19" s="57"/>
     </row>
-    <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="74" t="s">
         <v>20</v>
       </c>
@@ -1331,7 +1331,7 @@
       <c r="G20" s="56"/>
       <c r="H20" s="57"/>
     </row>
-    <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="75" t="s">
         <v>21</v>
       </c>
@@ -1370,26 +1370,26 @@
   <dimension ref="B2:U42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.26953125" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>22</v>
       </c>
@@ -1406,12 +1406,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1447,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1457,12 +1457,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C8" s="15" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1534,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C9" s="17" t="s">
         <v>33</v>
       </c>
@@ -1570,7 +1570,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C10" s="17" t="s">
         <v>11</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
         <v>34</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
         <v>12</v>
       </c>
@@ -1676,7 +1676,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
         <v>13</v>
       </c>
@@ -1711,7 +1711,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C14" s="17" t="s">
         <v>14</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
         <v>15</v>
       </c>
@@ -1781,7 +1781,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C16" s="19" t="s">
         <v>16</v>
       </c>
@@ -1816,7 +1816,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C17" s="19" t="s">
         <v>35</v>
       </c>
@@ -1851,12 +1851,12 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>18</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>19</v>
       </c>
@@ -1926,7 +1926,7 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>20</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>21</v>
       </c>
@@ -1996,12 +1996,12 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>61</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>54</v>
       </c>
@@ -2071,7 +2071,7 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
         <v>62</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2117,7 +2117,7 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B31" s="6" t="s">
         <v>100</v>
       </c>
@@ -2137,13 +2137,13 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C32" s="68">
         <f>INDEX(Outputs_Timeline!$D$3:$D$94,MATCH(Inputs!$C$1,Outputs_Timeline!$B$3:$B$94,0),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
         <v>99</v>
       </c>
@@ -2175,7 +2175,7 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2190,18 +2190,18 @@
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C38" s="7">
         <f>SUM(Outputs_Timeline!R:R)</f>
         <v>725305</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C39" s="53">
         <f>SUM(D34:H34)</f>
         <v>725305</v>
@@ -2209,17 +2209,17 @@
       <c r="D39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D41" s="2"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -2234,35 +2234,35 @@
   <dimension ref="B1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+    <col min="9" max="9" width="3.81640625" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F1" s="51" t="s">
         <v>83</v>
       </c>
       <c r="G1" s="51"/>
       <c r="H1" s="51"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D2" s="9" t="s">
         <v>68</v>
       </c>
@@ -2286,12 +2286,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="26"/>
@@ -2331,7 +2331,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>78</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C8" s="15" t="s">
         <v>3</v>
       </c>
@@ -2394,11 +2394,11 @@
         <v>0</v>
       </c>
       <c r="J8" s="16">
-        <f t="shared" ref="J7:J17" si="2">F8*$D8</f>
+        <f t="shared" ref="J8:J17" si="2">F8*$D8</f>
         <v>9720</v>
       </c>
       <c r="K8" s="16">
-        <f t="shared" ref="K7:K17" si="3">G8*$D8</f>
+        <f t="shared" ref="K8:K16" si="3">G8*$D8</f>
         <v>14580</v>
       </c>
       <c r="L8" s="16">
@@ -2406,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C9" s="17" t="s">
         <v>33</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C10" s="17" t="s">
         <v>11</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
         <v>34</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
         <v>12</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
         <v>13</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>17280</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C14" s="17" t="s">
         <v>14</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
         <v>15</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C16" s="19" t="s">
         <v>16</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C17" s="19" t="s">
         <v>35</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
@@ -2695,7 +2695,7 @@
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="G19" s="49" t="s">
         <v>80</v>
       </c>
@@ -2706,7 +2706,7 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -2714,7 +2714,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>79</v>
       </c>
@@ -2725,7 +2725,7 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C22" s="15" t="s">
         <v>2</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C23" s="28" t="s">
         <v>3</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="29">
-        <f t="shared" ref="J22:J32" si="9">F23*$D23</f>
+        <f t="shared" ref="J23:J32" si="9">F23*$D23</f>
         <v>0</v>
       </c>
       <c r="K23" s="29">
@@ -2793,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C24" s="17" t="s">
         <v>33</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C25" s="17" t="s">
         <v>11</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C26" s="17" t="s">
         <v>34</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C27" s="17" t="s">
         <v>12</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C28" s="17" t="s">
         <v>13</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>4977.7777777777792</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C29" s="17" t="s">
         <v>14</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>4977.7777777777792</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C30" s="19" t="s">
         <v>15</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C31" s="19" t="s">
         <v>16</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C32" s="28" t="s">
         <v>35</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
@@ -3100,7 +3100,7 @@
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
         <v>71</v>
       </c>
@@ -3111,7 +3111,7 @@
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C35" s="17" t="s">
         <v>18</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C36" s="17" t="s">
         <v>19</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C37" s="19" t="s">
         <v>20</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C38" s="19" t="s">
         <v>21</v>
       </c>
@@ -3235,12 +3235,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B40" s="6" t="s">
         <v>81</v>
       </c>
@@ -3251,7 +3251,7 @@
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C41" s="28" t="s">
         <v>18</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="50">
-        <f>(1-G41)*F35/SUM(F35,H35)</f>
+        <f>IFERROR((1-G41)*F35/SUM(F35,H35),0)</f>
         <v>0.5</v>
       </c>
       <c r="G41" s="50">
@@ -3268,7 +3268,7 @@
         <v>0.5</v>
       </c>
       <c r="H41" s="50">
-        <f>(1-G41)*H35/SUM(F35,H35)</f>
+        <f>IFERROR((1-G41)*H35/SUM(F35,H35),0)</f>
         <v>0</v>
       </c>
       <c r="J41" s="29">
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C42" s="17" t="s">
         <v>19</v>
       </c>
@@ -3293,15 +3293,15 @@
         <v>4000</v>
       </c>
       <c r="F42" s="30">
-        <f t="shared" ref="F42:F44" si="14">(1-G42)*F36/SUM(F36,H36)</f>
+        <f>IFERROR((1-G42)*F36/SUM(F36,H36),0)</f>
         <v>0.5</v>
       </c>
       <c r="G42" s="30">
-        <f t="shared" ref="G42:G44" si="15">MIN(1,G36+$H$19)</f>
+        <f t="shared" ref="G42:G44" si="14">MIN(1,G36+$H$19)</f>
         <v>0.5</v>
       </c>
       <c r="H42" s="30">
-        <f t="shared" ref="H42:H44" si="16">(1-G42)*H36/SUM(F36,H36)</f>
+        <f>IFERROR((1-G42)*H36/SUM(F36,H36),0)</f>
         <v>0</v>
       </c>
       <c r="J42" s="18">
@@ -3317,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C43" s="19" t="s">
         <v>20</v>
       </c>
@@ -3326,19 +3326,19 @@
         <v>0</v>
       </c>
       <c r="F43" s="31">
+        <f>IFERROR((1-G43)*F37/SUM(F37,H37),0)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G43" s="31">
         <f t="shared" si="14"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="G43" s="31">
-        <f t="shared" si="15"/>
         <v>0.7</v>
       </c>
       <c r="H43" s="31">
-        <f t="shared" si="16"/>
+        <f>IFERROR((1-G43)*H37/SUM(F37,H37),0)</f>
         <v>0</v>
       </c>
       <c r="J43" s="20">
-        <f t="shared" ref="J41:J44" si="17">F43*$D43</f>
+        <f t="shared" ref="J43:J44" si="15">F43*$D43</f>
         <v>0</v>
       </c>
       <c r="K43" s="20">
@@ -3350,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C44" s="19" t="s">
         <v>21</v>
       </c>
@@ -3359,19 +3359,19 @@
         <v>0</v>
       </c>
       <c r="F44" s="31">
+        <f>IFERROR((1-G44)*F38/SUM(F38,H38),0)</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G44" s="31">
         <f t="shared" si="14"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="G44" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="H44" s="31">
+        <f>IFERROR((1-G44)*H38/SUM(F38,H38),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="20">
         <f t="shared" si="15"/>
-        <v>0.7</v>
-      </c>
-      <c r="H44" s="31">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="20">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K44" s="20">
@@ -3383,12 +3383,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
         <v>60</v>
       </c>
@@ -3396,7 +3396,7 @@
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
         <v>61</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
         <v>54</v>
       </c>
@@ -3462,12 +3462,12 @@
         <v>-11000.091175512862</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B50" s="6" t="s">
         <v>62</v>
       </c>
@@ -3480,15 +3480,15 @@
         <v>82806.45453887622</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:L50" si="18">SUM(K47:K48, K35:K38, K7:K17,K22:K32,K41:K44)</f>
+        <f t="shared" ref="K50:L50" si="16">SUM(K47:K48, K35:K38, K7:K17,K22:K32,K41:K44)</f>
         <v>109373.08108108108</v>
       </c>
       <c r="L50" s="12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>27755.4643800427</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C51" s="21" t="s">
         <v>82</v>
       </c>
@@ -3500,12 +3500,12 @@
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53" s="6" t="s">
         <v>96</v>
       </c>
@@ -3526,27 +3526,27 @@
         <v>83266.393140128072</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D54" s="1"/>
       <c r="J54" s="54">
         <f>J53/$D$53</f>
         <v>0.37862604506604619</v>
       </c>
       <c r="K54" s="54">
-        <f t="shared" ref="K54:L54" si="19">K53/$D$53</f>
+        <f t="shared" ref="K54:L54" si="17">K53/$D$53</f>
         <v>0.5065720534716337</v>
       </c>
       <c r="L54" s="54">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.11480190146232008</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B57" s="27" t="s">
         <v>77</v>
       </c>
@@ -3561,7 +3561,7 @@
       <c r="K57" s="22"/>
       <c r="L57" s="22"/>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B58" s="27"/>
       <c r="C58" s="21" t="s">
         <v>18</v>
@@ -3585,19 +3585,19 @@
       </c>
       <c r="I58" s="21"/>
       <c r="J58" s="25">
-        <f t="shared" ref="J58:L61" si="20">F58*$D58</f>
+        <f t="shared" ref="J58:L61" si="18">F58*$D58</f>
         <v>0</v>
       </c>
       <c r="K58" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L58" s="25">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B59" s="27"/>
       <c r="C59" s="21" t="s">
         <v>19</v>
@@ -3612,28 +3612,28 @@
         <v>0.37975090959977603</v>
       </c>
       <c r="G59" s="24">
-        <f t="shared" ref="G59:H59" si="21">IFERROR(SUM(K$36,K$9:K$14,K$42,K$24:K$29)/SUM($J$36:$L$36,$J$9:$L$14,$J$42:$L$42,$J$24:$L$29),0)</f>
+        <f t="shared" ref="G59:H59" si="19">IFERROR(SUM(K$36,K$9:K$14,K$42,K$24:K$29)/SUM($J$36:$L$36,$J$9:$L$14,$J$42:$L$42,$J$24:$L$29),0)</f>
         <v>0.37619647355163727</v>
       </c>
       <c r="H59" s="24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.24405261684858667</v>
       </c>
       <c r="I59" s="21"/>
       <c r="J59" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>60304.444444444431</v>
       </c>
       <c r="K59" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>59740</v>
       </c>
       <c r="L59" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>38755.555555555562</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B60" s="27"/>
       <c r="C60" s="21" t="s">
         <v>20</v>
@@ -3657,19 +3657,19 @@
       </c>
       <c r="I60" s="21"/>
       <c r="J60" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K60" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L60" s="25">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B61" s="27"/>
       <c r="C61" s="21" t="s">
         <v>21</v>
@@ -3693,15 +3693,15 @@
       </c>
       <c r="I61" s="21"/>
       <c r="J61" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="K61" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L61" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -3719,26 +3719,26 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W9" sqref="W9"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="64" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="64" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="64" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="64" customWidth="1"/>
-    <col min="8" max="11" width="8.7109375" style="67"/>
-    <col min="12" max="12" width="5.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="67" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="8.7109375" style="67"/>
-    <col min="17" max="17" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.453125" style="64" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="64" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.54296875" style="64" customWidth="1"/>
+    <col min="8" max="11" width="8.7265625" style="67"/>
+    <col min="12" max="12" width="5.453125" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="67" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="8.7265625" style="67"/>
+    <col min="17" max="17" width="3.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.35">
       <c r="F1" s="69">
         <f>COUNTIF(F3:F94,"&gt;0")</f>
         <v>36</v>
@@ -3762,7 +3762,7 @@
       <c r="T1" s="65"/>
       <c r="U1" s="65"/>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B2" s="63" t="s">
         <v>87</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="64">
         <v>42917</v>
       </c>
@@ -3867,7 +3867,7 @@
       <c r="T3" s="67"/>
       <c r="U3" s="67"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B4" s="64">
         <f>EDATE(B3,1)</f>
         <v>42948</v>
@@ -3917,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" s="64">
         <f t="shared" ref="B5:B68" si="0">EDATE(B4,1)</f>
         <v>42979</v>
@@ -3983,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="64">
         <f t="shared" si="0"/>
         <v>43009</v>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B7" s="64">
         <f t="shared" si="0"/>
         <v>43040</v>
@@ -4115,7 +4115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B8" s="64">
         <f t="shared" si="0"/>
         <v>43070</v>
@@ -4181,7 +4181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B9" s="64">
         <f t="shared" si="0"/>
         <v>43101</v>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" s="64">
         <f t="shared" si="0"/>
         <v>43132</v>
@@ -4313,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" s="64">
         <f t="shared" si="0"/>
         <v>43160</v>
@@ -4379,7 +4379,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B12" s="64">
         <f t="shared" si="0"/>
         <v>43191</v>
@@ -4445,7 +4445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B13" s="64">
         <f t="shared" si="0"/>
         <v>43221</v>
@@ -4511,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" s="64">
         <f t="shared" si="0"/>
         <v>43252</v>
@@ -4577,7 +4577,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" s="64">
         <f t="shared" si="0"/>
         <v>43282</v>
@@ -4643,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B16" s="64">
         <f t="shared" si="0"/>
         <v>43313</v>
@@ -4709,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B17" s="64">
         <f t="shared" si="0"/>
         <v>43344</v>
@@ -4775,7 +4775,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" s="64">
         <f t="shared" si="0"/>
         <v>43374</v>
@@ -4841,7 +4841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="64">
         <f t="shared" si="0"/>
         <v>43405</v>
@@ -4907,7 +4907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B20" s="64">
         <f t="shared" si="0"/>
         <v>43435</v>
@@ -4973,7 +4973,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B21" s="64">
         <f t="shared" si="0"/>
         <v>43466</v>
@@ -5039,7 +5039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B22" s="64">
         <f t="shared" si="0"/>
         <v>43497</v>
@@ -5105,7 +5105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B23" s="64">
         <f t="shared" si="0"/>
         <v>43525</v>
@@ -5171,7 +5171,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B24" s="64">
         <f t="shared" si="0"/>
         <v>43556</v>
@@ -5237,7 +5237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B25" s="64">
         <f t="shared" si="0"/>
         <v>43586</v>
@@ -5303,7 +5303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B26" s="64">
         <f t="shared" si="0"/>
         <v>43617</v>
@@ -5369,7 +5369,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B27" s="64">
         <f t="shared" si="0"/>
         <v>43647</v>
@@ -5435,7 +5435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B28" s="64">
         <f t="shared" si="0"/>
         <v>43678</v>
@@ -5501,7 +5501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B29" s="64">
         <f t="shared" si="0"/>
         <v>43709</v>
@@ -5567,7 +5567,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B30" s="64">
         <f t="shared" si="0"/>
         <v>43739</v>
@@ -5633,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B31" s="64">
         <f t="shared" si="0"/>
         <v>43770</v>
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B32" s="64">
         <f t="shared" si="0"/>
         <v>43800</v>
@@ -5765,7 +5765,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B33" s="64">
         <f t="shared" si="0"/>
         <v>43831</v>
@@ -5831,7 +5831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B34" s="64">
         <f t="shared" si="0"/>
         <v>43862</v>
@@ -5897,7 +5897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B35" s="64">
         <f t="shared" si="0"/>
         <v>43891</v>
@@ -5963,7 +5963,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B36" s="64">
         <f t="shared" si="0"/>
         <v>43922</v>
@@ -6029,7 +6029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B37" s="64">
         <f t="shared" si="0"/>
         <v>43952</v>
@@ -6095,7 +6095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B38" s="64">
         <f t="shared" si="0"/>
         <v>43983</v>
@@ -6161,7 +6161,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B39" s="64">
         <f t="shared" si="0"/>
         <v>44013</v>
@@ -6227,7 +6227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B40" s="64">
         <f t="shared" si="0"/>
         <v>44044</v>
@@ -6293,7 +6293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B41" s="64">
         <f t="shared" si="0"/>
         <v>44075</v>
@@ -6359,7 +6359,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B42" s="64">
         <f t="shared" si="0"/>
         <v>44105</v>
@@ -6425,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B43" s="64">
         <f t="shared" si="0"/>
         <v>44136</v>
@@ -6491,7 +6491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B44" s="64">
         <f t="shared" si="0"/>
         <v>44166</v>
@@ -6557,7 +6557,7 @@
         <v>6938.8660950106751</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B45" s="64">
         <f t="shared" si="0"/>
         <v>44197</v>
@@ -6623,7 +6623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B46" s="64">
         <f t="shared" si="0"/>
         <v>44228</v>
@@ -6689,7 +6689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B47" s="64">
         <f t="shared" si="0"/>
         <v>44256</v>
@@ -6755,7 +6755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B48" s="64">
         <f t="shared" si="0"/>
         <v>44287</v>
@@ -6821,7 +6821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B49" s="64">
         <f t="shared" si="0"/>
         <v>44317</v>
@@ -6887,7 +6887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B50" s="64">
         <f t="shared" si="0"/>
         <v>44348</v>
@@ -6953,7 +6953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B51" s="64">
         <f t="shared" si="0"/>
         <v>44378</v>
@@ -7019,7 +7019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B52" s="64">
         <f t="shared" si="0"/>
         <v>44409</v>
@@ -7085,7 +7085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B53" s="64">
         <f t="shared" si="0"/>
         <v>44440</v>
@@ -7151,7 +7151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B54" s="64">
         <f t="shared" si="0"/>
         <v>44470</v>
@@ -7217,7 +7217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B55" s="64">
         <f t="shared" si="0"/>
         <v>44501</v>
@@ -7283,7 +7283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B56" s="64">
         <f t="shared" si="0"/>
         <v>44531</v>
@@ -7349,7 +7349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B57" s="64">
         <f t="shared" si="0"/>
         <v>44562</v>
@@ -7415,7 +7415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B58" s="64">
         <f t="shared" si="0"/>
         <v>44593</v>
@@ -7481,7 +7481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B59" s="64">
         <f t="shared" si="0"/>
         <v>44621</v>
@@ -7547,7 +7547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B60" s="64">
         <f t="shared" si="0"/>
         <v>44652</v>
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B61" s="64">
         <f t="shared" si="0"/>
         <v>44682</v>
@@ -7679,7 +7679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B62" s="64">
         <f t="shared" si="0"/>
         <v>44713</v>
@@ -7745,7 +7745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B63" s="64">
         <f t="shared" si="0"/>
         <v>44743</v>
@@ -7811,7 +7811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B64" s="64">
         <f t="shared" si="0"/>
         <v>44774</v>
@@ -7877,7 +7877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B65" s="64">
         <f t="shared" si="0"/>
         <v>44805</v>
@@ -7943,7 +7943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B66" s="64">
         <f t="shared" si="0"/>
         <v>44835</v>
@@ -8009,7 +8009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B67" s="64">
         <f t="shared" si="0"/>
         <v>44866</v>
@@ -8075,7 +8075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B68" s="64">
         <f t="shared" si="0"/>
         <v>44896</v>
@@ -8141,7 +8141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B69" s="64">
         <f t="shared" ref="B69:B94" si="6">EDATE(B68,1)</f>
         <v>44927</v>
@@ -8207,7 +8207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B70" s="64">
         <f t="shared" si="6"/>
         <v>44958</v>
@@ -8273,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B71" s="64">
         <f t="shared" si="6"/>
         <v>44986</v>
@@ -8339,7 +8339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B72" s="64">
         <f t="shared" si="6"/>
         <v>45017</v>
@@ -8405,7 +8405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B73" s="64">
         <f t="shared" si="6"/>
         <v>45047</v>
@@ -8471,7 +8471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B74" s="64">
         <f t="shared" si="6"/>
         <v>45078</v>
@@ -8537,7 +8537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B75" s="64">
         <f t="shared" si="6"/>
         <v>45108</v>
@@ -8603,7 +8603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B76" s="64">
         <f t="shared" si="6"/>
         <v>45139</v>
@@ -8669,7 +8669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B77" s="64">
         <f t="shared" si="6"/>
         <v>45170</v>
@@ -8735,7 +8735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B78" s="64">
         <f t="shared" si="6"/>
         <v>45200</v>
@@ -8801,7 +8801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B79" s="64">
         <f t="shared" si="6"/>
         <v>45231</v>
@@ -8867,7 +8867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B80" s="64">
         <f t="shared" si="6"/>
         <v>45261</v>
@@ -8933,7 +8933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B81" s="64">
         <f t="shared" si="6"/>
         <v>45292</v>
@@ -8999,7 +8999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B82" s="64">
         <f t="shared" si="6"/>
         <v>45323</v>
@@ -9065,7 +9065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B83" s="64">
         <f t="shared" si="6"/>
         <v>45352</v>
@@ -9131,7 +9131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B84" s="64">
         <f t="shared" si="6"/>
         <v>45383</v>
@@ -9197,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B85" s="64">
         <f t="shared" si="6"/>
         <v>45413</v>
@@ -9263,7 +9263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B86" s="64">
         <f t="shared" si="6"/>
         <v>45444</v>
@@ -9329,7 +9329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B87" s="64">
         <f t="shared" si="6"/>
         <v>45474</v>
@@ -9395,7 +9395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B88" s="64">
         <f t="shared" si="6"/>
         <v>45505</v>
@@ -9461,7 +9461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B89" s="64">
         <f t="shared" si="6"/>
         <v>45536</v>
@@ -9527,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B90" s="64">
         <f t="shared" si="6"/>
         <v>45566</v>
@@ -9593,7 +9593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B91" s="64">
         <f t="shared" si="6"/>
         <v>45597</v>
@@ -9659,7 +9659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B92" s="64">
         <f t="shared" si="6"/>
         <v>45627</v>
@@ -9725,7 +9725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B93" s="64">
         <f t="shared" si="6"/>
         <v>45658</v>
@@ -9791,7 +9791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B94" s="64">
         <f t="shared" si="6"/>
         <v>45689</v>
@@ -9875,19 +9875,19 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J99" sqref="J99"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" customWidth="1"/>
-    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="15" width="18" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>22</v>
       </c>
@@ -9919,12 +9919,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -9949,14 +9949,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>46</v>
       </c>
@@ -9981,19 +9981,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C10" s="15" t="s">
         <v>3</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
         <v>33</v>
       </c>
@@ -10068,7 +10068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
         <v>11</v>
       </c>
@@ -10093,7 +10093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
         <v>34</v>
       </c>
@@ -10118,7 +10118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
@@ -10143,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C15" s="17" t="s">
         <v>13</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C16" s="17" t="s">
         <v>14</v>
       </c>
@@ -10193,7 +10193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C17" s="19" t="s">
         <v>15</v>
       </c>
@@ -10218,7 +10218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C19" s="19" t="s">
         <v>35</v>
       </c>
@@ -10268,12 +10268,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C22" s="15" t="s">
         <v>2</v>
       </c>
@@ -10298,7 +10298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C23" s="28" t="s">
         <v>3</v>
       </c>
@@ -10318,7 +10318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C24" s="17" t="s">
         <v>33</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C25" s="17" t="s">
         <v>11</v>
       </c>
@@ -10368,7 +10368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C26" s="17" t="s">
         <v>34</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C27" s="17" t="s">
         <v>12</v>
       </c>
@@ -10418,7 +10418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C28" s="17" t="s">
         <v>13</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C29" s="17" t="s">
         <v>14</v>
       </c>
@@ -10468,7 +10468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C30" s="19" t="s">
         <v>15</v>
       </c>
@@ -10493,7 +10493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C31" s="19" t="s">
         <v>16</v>
       </c>
@@ -10518,7 +10518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C32" s="28" t="s">
         <v>35</v>
       </c>
@@ -10538,19 +10538,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C35" s="15" t="s">
         <v>2</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C36" s="15" t="s">
         <v>3</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C37" s="17" t="s">
         <v>33</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C38" s="17" t="s">
         <v>11</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C39" s="17" t="s">
         <v>34</v>
       </c>
@@ -10675,7 +10675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C40" s="17" t="s">
         <v>12</v>
       </c>
@@ -10700,7 +10700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C41" s="17" t="s">
         <v>13</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C42" s="17" t="s">
         <v>14</v>
       </c>
@@ -10750,7 +10750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C43" s="19" t="s">
         <v>15</v>
       </c>
@@ -10775,7 +10775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C44" s="19" t="s">
         <v>16</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C45" s="19" t="s">
         <v>35</v>
       </c>
@@ -10825,12 +10825,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C48" s="15" t="s">
         <v>2</v>
       </c>
@@ -10855,7 +10855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C49" s="28" t="s">
         <v>3</v>
       </c>
@@ -10875,7 +10875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C50" s="17" t="s">
         <v>33</v>
       </c>
@@ -10900,7 +10900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C51" s="17" t="s">
         <v>11</v>
       </c>
@@ -10925,7 +10925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C52" s="17" t="s">
         <v>34</v>
       </c>
@@ -10950,7 +10950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C53" s="17" t="s">
         <v>12</v>
       </c>
@@ -10975,7 +10975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C54" s="17" t="s">
         <v>13</v>
       </c>
@@ -11000,7 +11000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C55" s="17" t="s">
         <v>14</v>
       </c>
@@ -11025,7 +11025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C56" s="19" t="s">
         <v>15</v>
       </c>
@@ -11050,7 +11050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C57" s="19" t="s">
         <v>16</v>
       </c>
@@ -11075,7 +11075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C58" s="28" t="s">
         <v>35</v>
       </c>
@@ -11095,12 +11095,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B60" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C61" s="17" t="s">
         <v>18</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C62" s="17" t="s">
         <v>19</v>
       </c>
@@ -11190,7 +11190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C63" s="19" t="s">
         <v>20</v>
       </c>
@@ -11235,7 +11235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C64" s="19" t="s">
         <v>21</v>
       </c>
@@ -11280,12 +11280,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B66" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C67" s="28" t="s">
         <v>18</v>
       </c>
@@ -11325,7 +11325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C68" s="17" t="s">
         <v>19</v>
       </c>
@@ -11350,7 +11350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C69" s="19" t="s">
         <v>20</v>
       </c>
@@ -11375,7 +11375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C70" s="19" t="s">
         <v>21</v>
       </c>
@@ -11400,19 +11400,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B72" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C73" s="17" t="s">
         <v>18</v>
       </c>
@@ -11437,7 +11437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C74" s="17" t="s">
         <v>19</v>
       </c>
@@ -11462,7 +11462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C75" s="19" t="s">
         <v>20</v>
       </c>
@@ -11487,7 +11487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C76" s="19" t="s">
         <v>21</v>
       </c>
@@ -11512,12 +11512,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B78" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C79" s="28" t="s">
         <v>18</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C80" s="17" t="s">
         <v>19</v>
       </c>
@@ -11582,7 +11582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C81" s="19" t="s">
         <v>20</v>
       </c>
@@ -11607,7 +11607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C82" s="19" t="s">
         <v>21</v>
       </c>
@@ -11632,12 +11632,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B84" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C85" t="s">
         <v>38</v>
       </c>
@@ -11662,7 +11662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C86" t="s">
         <v>39</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B88" s="6" t="s">
         <v>48</v>
       </c>
@@ -11712,10 +11712,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B90" s="6" t="s">
         <v>66</v>
       </c>
@@ -11740,7 +11740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B92" s="6" t="s">
         <v>57</v>
       </c>
@@ -11765,7 +11765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B95" s="27"/>
       <c r="C95" s="21" t="s">
         <v>67</v>
@@ -11791,7 +11791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B96" s="27"/>
       <c r="D96" s="21">
         <v>0.1</v>
@@ -11809,7 +11809,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B97" s="27"/>
       <c r="D97" s="21">
         <f>SUM(D95:D96)</f>
@@ -11832,7 +11832,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="98" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B98" s="27"/>
       <c r="D98" s="21">
         <f>_xlfn.RANK.EQ(D97, $D$97:$H$97, 5)</f>
@@ -11855,16 +11855,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B99" s="27"/>
     </row>
-    <row r="100" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B100" s="27"/>
       <c r="C100" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="101" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B101" s="27"/>
       <c r="D101" s="21" t="s">
         <v>42</v>
@@ -11874,7 +11874,7 @@
         <v>-54315</v>
       </c>
     </row>
-    <row r="102" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B102" s="27"/>
       <c r="D102" s="21" t="s">
         <v>43</v>
@@ -11884,7 +11884,7 @@
         <v>-32850</v>
       </c>
     </row>
-    <row r="103" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B103" s="27"/>
       <c r="D103" s="21" t="s">
         <v>55</v>
@@ -11894,7 +11894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B104" s="27"/>
       <c r="D104" s="21" t="s">
         <v>56</v>
@@ -11904,7 +11904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F108" s="2"/>
     </row>
   </sheetData>
@@ -11917,23 +11917,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.140625" customWidth="1"/>
-    <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" customWidth="1"/>
+    <col min="2" max="2" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.1796875" customWidth="1"/>
+    <col min="8" max="8" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C2" s="49" t="s">
         <v>6</v>
       </c>
@@ -11941,7 +11939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -11956,7 +11954,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -11974,7 +11972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="E5" s="6" t="s">
         <v>29</v>
       </c>
@@ -11985,7 +11983,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>31</v>
       </c>
@@ -12005,7 +12003,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
         <v>32</v>
       </c>
@@ -12019,14 +12017,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C8" s="44"/>
       <c r="D8" s="40"/>
       <c r="H8" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C9" s="47" t="s">
         <v>44</v>
       </c>
@@ -12040,7 +12038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
         <v>33</v>
       </c>
@@ -12057,7 +12055,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
@@ -12074,7 +12072,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
         <v>34</v>
       </c>
@@ -12085,7 +12083,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
         <v>12</v>
       </c>
@@ -12097,7 +12095,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
         <v>13</v>
       </c>
@@ -12114,7 +12112,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
         <v>14</v>
       </c>
@@ -12131,7 +12129,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
         <v>15</v>
       </c>
@@ -12144,7 +12142,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
         <v>16</v>
       </c>
@@ -12155,7 +12153,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
         <v>35</v>
       </c>
@@ -12166,11 +12164,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C19" s="44"/>
       <c r="D19" s="40"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="17" t="s">
         <v>18</v>
       </c>
@@ -12181,7 +12179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
         <v>19</v>
       </c>
@@ -12192,7 +12190,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="19" t="s">
         <v>20</v>
       </c>
@@ -12203,7 +12201,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Fix ACO Insights basic calc.
Do this because it was fixed by column.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
@@ -1291,7 +1291,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="56" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="F18" s="56" t="s">
         <v>45</v>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F19" s="56" t="s">
         <v>4</v>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="E9" s="18">
         <f>SUM(Calcs!E37, Calcs!E50)</f>
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="F9" s="18">
         <f>SUM(Calcs!F37, Calcs!F50)</f>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="E10" s="18">
         <f>SUM(Calcs!E38, Calcs!E51)</f>
-        <v>0</v>
+        <v>8300</v>
       </c>
       <c r="F10" s="18">
         <f>SUM(Calcs!F38, Calcs!F51)</f>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="E11" s="18">
         <f>SUM(Calcs!E39, Calcs!E52)</f>
-        <v>0</v>
+        <v>4900</v>
       </c>
       <c r="F11" s="18">
         <f>SUM(Calcs!F39, Calcs!F52)</f>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="E12" s="18">
         <f>SUM(Calcs!E40, Calcs!E53)</f>
-        <v>0</v>
+        <v>4900</v>
       </c>
       <c r="F12" s="18">
         <f>SUM(Calcs!F40, Calcs!F53)</f>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="E20" s="1">
         <f>SUM(Calcs!E61, Calcs!E67)</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="F20" s="1">
         <f>SUM(Calcs!F61, Calcs!F67)</f>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="E21" s="1">
         <f>SUM(Calcs!E62, Calcs!E68)</f>
-        <v>59600</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1">
         <f>SUM(Calcs!F62, Calcs!F68)</f>
@@ -2046,11 +2046,11 @@
       </c>
       <c r="E27" s="1">
         <f>Calcs!E90</f>
-        <v>0</v>
+        <v>-41895</v>
       </c>
       <c r="F27" s="1">
         <f>Calcs!F90</f>
-        <v>-54315</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
         <f>Calcs!G90</f>
@@ -2081,11 +2081,11 @@
       </c>
       <c r="E29" s="7">
         <f t="shared" ref="E29:H29" si="0">SUM(E7:E17, E20:E23, E26:E27)</f>
-        <v>120700</v>
+        <v>51205</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="0"/>
-        <v>66385</v>
+        <v>120700</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" si="0"/>
@@ -2153,11 +2153,11 @@
       </c>
       <c r="E34" s="7">
         <f>(E29/12*Inputs!$C$2+E4)*$C$32</f>
-        <v>394850</v>
+        <v>186365</v>
       </c>
       <c r="F34" s="7">
         <f>(F29/12*Inputs!$C$2+F4)*$C$32</f>
-        <v>231905</v>
+        <v>394850</v>
       </c>
       <c r="G34" s="7">
         <f>(G29/12*Inputs!$C$2+G4)*$C$32</f>
@@ -2198,13 +2198,13 @@
     <row r="38" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C38" s="7">
         <f>SUM(Outputs_Timeline!R:R)</f>
-        <v>725305</v>
+        <v>679765</v>
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C39" s="53">
         <f>SUM(D34:H34)</f>
-        <v>725305</v>
+        <v>679765</v>
       </c>
       <c r="D39" s="1"/>
       <c r="G39" s="1"/>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="D13" s="18">
         <f>SUM(Calcs!D15:H15)</f>
-        <v>21600</v>
+        <v>14400</v>
       </c>
       <c r="F13" s="33">
         <v>0.1</v>
@@ -2552,15 +2552,15 @@
       </c>
       <c r="J13" s="18">
         <f t="shared" si="2"/>
-        <v>2160</v>
+        <v>1440</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="3"/>
-        <v>2160</v>
+        <v>1440</v>
       </c>
       <c r="L13" s="18">
         <f t="shared" si="1"/>
-        <v>17280</v>
+        <v>11520</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="D14" s="18">
         <f>SUM(Calcs!D16:H16)</f>
-        <v>14400</v>
+        <v>9600</v>
       </c>
       <c r="F14" s="33">
         <v>0.1</v>
@@ -2583,15 +2583,15 @@
       </c>
       <c r="J14" s="18">
         <f t="shared" si="2"/>
-        <v>1440</v>
+        <v>960</v>
       </c>
       <c r="K14" s="18">
         <f t="shared" si="3"/>
-        <v>1440</v>
+        <v>960</v>
       </c>
       <c r="L14" s="18">
         <f t="shared" si="1"/>
-        <v>11520</v>
+        <v>7680</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="D28" s="18">
         <f>SUM(Calcs!D28:H28)</f>
-        <v>7000.0000000000009</v>
+        <v>3500.0000000000005</v>
       </c>
       <c r="F28" s="37">
         <f t="shared" si="7"/>
@@ -2949,15 +2949,15 @@
       </c>
       <c r="J28" s="18">
         <f t="shared" si="9"/>
-        <v>622.2222222222224</v>
+        <v>311.1111111111112</v>
       </c>
       <c r="K28" s="18">
         <f t="shared" si="5"/>
-        <v>1400.0000000000002</v>
+        <v>700.00000000000011</v>
       </c>
       <c r="L28" s="18">
         <f t="shared" si="6"/>
-        <v>4977.7777777777792</v>
+        <v>2488.8888888888896</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="D29" s="18">
         <f>SUM(Calcs!D29:H29)</f>
-        <v>7000.0000000000009</v>
+        <v>3500.0000000000005</v>
       </c>
       <c r="F29" s="37">
         <f t="shared" si="7"/>
@@ -2982,15 +2982,15 @@
       </c>
       <c r="J29" s="18">
         <f t="shared" si="9"/>
-        <v>622.2222222222224</v>
+        <v>311.1111111111112</v>
       </c>
       <c r="K29" s="18">
         <f t="shared" si="5"/>
-        <v>1400.0000000000002</v>
+        <v>700.00000000000011</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" si="6"/>
-        <v>4977.7777777777792</v>
+        <v>2488.8888888888896</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
@@ -3117,7 +3117,7 @@
       </c>
       <c r="D35" s="18">
         <f>SUM(Calcs!D73:H73)</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="F35" s="33">
         <v>0.6</v>
@@ -3131,11 +3131,11 @@
       </c>
       <c r="J35" s="18">
         <f>F35*$D35</f>
-        <v>0</v>
+        <v>6120</v>
       </c>
       <c r="K35" s="18">
         <f t="shared" ref="J35:L38" si="11">G35*$D35</f>
-        <v>0</v>
+        <v>4080</v>
       </c>
       <c r="L35" s="18">
         <f t="shared" si="11"/>
@@ -3148,7 +3148,7 @@
       </c>
       <c r="D36" s="18">
         <f>SUM(Calcs!D74:H74)</f>
-        <v>50400</v>
+        <v>33600</v>
       </c>
       <c r="F36" s="33">
         <v>0.6</v>
@@ -3162,11 +3162,11 @@
       </c>
       <c r="J36" s="18">
         <f t="shared" si="11"/>
-        <v>30240</v>
+        <v>20160</v>
       </c>
       <c r="K36" s="18">
         <f t="shared" si="11"/>
-        <v>20160</v>
+        <v>13440</v>
       </c>
       <c r="L36" s="18">
         <f t="shared" si="11"/>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="D42" s="18">
         <f>SUM(Calcs!D80:H80)</f>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="F42" s="30">
         <f>IFERROR((1-G42)*F36/SUM(F36,H36),0)</f>
@@ -3306,11 +3306,11 @@
       </c>
       <c r="J42" s="18">
         <f>F42*$D42</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="K42" s="18">
         <f t="shared" si="12"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="L42" s="18">
         <f t="shared" si="13"/>
@@ -3406,15 +3406,15 @@
       </c>
       <c r="F47" s="8">
         <f>IFERROR(SUM(J58:J61)/SUM($J$58:$L$61), 0)</f>
-        <v>0.37975090959977603</v>
+        <v>0.41116990076936893</v>
       </c>
       <c r="G47" s="8">
         <f>IFERROR(SUM(K58:K61)/SUM($J$58:$L$61), 0)</f>
-        <v>0.37619647355163727</v>
+        <v>0.40764379712028043</v>
       </c>
       <c r="H47" s="8">
         <f>IFERROR(SUM(L58:L61)/SUM($J$58:$L$61), 0)</f>
-        <v>0.24405261684858667</v>
+        <v>0.18118630211035067</v>
       </c>
       <c r="J47" s="12">
         <f>F47*$D$47</f>
@@ -3435,31 +3435,31 @@
       </c>
       <c r="D48" s="1">
         <f>SUM(Outputs_External!D27:'Outputs_External'!H27)</f>
-        <v>-87165</v>
+        <v>-74745</v>
       </c>
       <c r="F48" s="3">
         <f>IFERROR(SUM(J7:J47)/SUM(J7:L47), 0)</f>
-        <v>0.3765042150584319</v>
+        <v>0.38941761081295961</v>
       </c>
       <c r="G48" s="3">
         <f>IFERROR(SUM(K7:K47)/SUM(J7:L47), 0)</f>
-        <v>0.49729729729729732</v>
+        <v>0.52407871198568878</v>
       </c>
       <c r="H48" s="3">
         <f>1-F48-G48</f>
-        <v>0.12619848764427077</v>
+        <v>8.6503677201351548E-2</v>
       </c>
       <c r="J48" s="12">
         <f>F48*$D$48</f>
-        <v>-32817.989905568218</v>
+        <v>-29107.019320214666</v>
       </c>
       <c r="K48" s="12">
         <f>G48*$D$48</f>
-        <v>-43346.91891891892</v>
+        <v>-39172.26332737031</v>
       </c>
       <c r="L48" s="12">
         <f>H48*$D$48</f>
-        <v>-11000.091175512862</v>
+        <v>-6465.7173524150212</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.35">
@@ -3473,19 +3473,19 @@
       </c>
       <c r="D50" s="1">
         <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
-        <v>219935</v>
+        <v>204755</v>
       </c>
       <c r="J50" s="12">
         <f>SUM(J47:J48, J35:J38, J7:J17,J22:J32,J41:J44)</f>
-        <v>82806.45453887622</v>
+        <v>79735.202902007557</v>
       </c>
       <c r="K50" s="12">
         <f t="shared" ref="K50:L50" si="16">SUM(K47:K48, K35:K38, K7:K17,K22:K32,K41:K44)</f>
-        <v>109373.08108108108</v>
+        <v>107307.73667262969</v>
       </c>
       <c r="L50" s="12">
         <f t="shared" si="16"/>
-        <v>27755.4643800427</v>
+        <v>17712.060425362761</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.35">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="D51" s="23">
         <f>SUM(J50:L50)</f>
-        <v>219935</v>
+        <v>204755</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
@@ -3511,34 +3511,34 @@
       </c>
       <c r="D53" s="1">
         <f>SUM(Outputs_Timeline!R:R)</f>
-        <v>725305</v>
+        <v>679765</v>
       </c>
       <c r="J53" s="12">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>274619.36361662863</v>
+        <v>265405.60870602273</v>
       </c>
       <c r="K53" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>367419.24324324331</v>
+        <v>361223.21001788904</v>
       </c>
       <c r="L53" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
-        <v>83266.393140128072</v>
+        <v>53136.181276088268</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D54" s="1"/>
       <c r="J54" s="54">
         <f>J53/$D$53</f>
-        <v>0.37862604506604619</v>
+        <v>0.39043729628036561</v>
       </c>
       <c r="K54" s="54">
         <f t="shared" ref="K54:L54" si="17">K53/$D$53</f>
-        <v>0.5065720534716337</v>
+        <v>0.53139424656740053</v>
       </c>
       <c r="L54" s="54">
         <f t="shared" si="17"/>
-        <v>0.11480190146232008</v>
+        <v>7.8168457152233889E-2</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.35">
@@ -3568,7 +3568,7 @@
       </c>
       <c r="D58" s="23">
         <f>SUM(Calcs!D61:H61)+SUM(Calcs!D67:H67)</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="E58" s="21"/>
       <c r="F58" s="24">
@@ -3586,11 +3586,11 @@
       <c r="I58" s="21"/>
       <c r="J58" s="25">
         <f t="shared" ref="J58:L61" si="18">F58*$D58</f>
-        <v>0</v>
+        <v>6120</v>
       </c>
       <c r="K58" s="25">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>4080</v>
       </c>
       <c r="L58" s="25">
         <f t="shared" si="18"/>
@@ -3604,33 +3604,33 @@
       </c>
       <c r="D59" s="23">
         <f>SUM(Calcs!D62:H62)+SUM(Calcs!D68:H68)</f>
-        <v>158800</v>
+        <v>99200</v>
       </c>
       <c r="E59" s="21"/>
       <c r="F59" s="24">
         <f>IFERROR(SUM(J$36,J$9:J$14,J$42,J$24:J$29)/SUM($J$36:$L$36,$J$9:$L$14,$J$42:$L$42,$J$24:$L$29),0)</f>
-        <v>0.37975090959977603</v>
+        <v>0.39175390266299354</v>
       </c>
       <c r="G59" s="24">
         <f t="shared" ref="G59:H59" si="19">IFERROR(SUM(K$36,K$9:K$14,K$42,K$24:K$29)/SUM($J$36:$L$36,$J$9:$L$14,$J$42:$L$42,$J$24:$L$29),0)</f>
-        <v>0.37619647355163727</v>
+        <v>0.4084297520661157</v>
       </c>
       <c r="H59" s="24">
         <f t="shared" si="19"/>
-        <v>0.24405261684858667</v>
+        <v>0.19981634527089076</v>
       </c>
       <c r="I59" s="21"/>
       <c r="J59" s="25">
         <f t="shared" si="18"/>
-        <v>60304.444444444431</v>
+        <v>38861.987144168961</v>
       </c>
       <c r="K59" s="25">
         <f t="shared" si="18"/>
-        <v>59740</v>
+        <v>40516.231404958678</v>
       </c>
       <c r="L59" s="25">
         <f t="shared" si="18"/>
-        <v>38755.555555555562</v>
+        <v>19821.781450872364</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.35">
@@ -4216,19 +4216,19 @@
       </c>
       <c r="M9" s="67">
         <f>$F9*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N9" s="67">
         <f>$F9*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O9" s="67">
         <f>$F9*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P9" s="67">
         <f>$F9*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R9" s="67">
         <f t="shared" si="2"/>
@@ -4282,19 +4282,19 @@
       </c>
       <c r="M10" s="67">
         <f>$F10*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N10" s="67">
         <f>$F10*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O10" s="67">
         <f>$F10*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P10" s="67">
         <f>$F10*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R10" s="67">
         <f t="shared" si="2"/>
@@ -4348,35 +4348,35 @@
       </c>
       <c r="M11" s="67">
         <f>$F11*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N11" s="67">
         <f>$F11*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O11" s="67">
         <f>$F11*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P11" s="67">
         <f>$F11*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R11" s="67">
         <f t="shared" si="2"/>
-        <v>120483.75000000001</v>
+        <v>116688.75000000001</v>
       </c>
       <c r="S11" s="67">
         <f t="shared" si="3"/>
-        <v>46901.613634719062</v>
+        <v>46133.800725501889</v>
       </c>
       <c r="T11" s="67">
         <f t="shared" si="4"/>
-        <v>66643.270270270266</v>
+        <v>66126.93416815743</v>
       </c>
       <c r="U11" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.35">
@@ -4414,19 +4414,19 @@
       </c>
       <c r="M12" s="67">
         <f>$F12*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N12" s="67">
         <f>$F12*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O12" s="67">
         <f>$F12*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P12" s="67">
         <f>$F12*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R12" s="67">
         <f t="shared" si="2"/>
@@ -4480,19 +4480,19 @@
       </c>
       <c r="M13" s="67">
         <f>$F13*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N13" s="67">
         <f>$F13*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O13" s="67">
         <f>$F13*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P13" s="67">
         <f>$F13*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R13" s="67">
         <f t="shared" si="2"/>
@@ -4546,35 +4546,35 @@
       </c>
       <c r="M14" s="67">
         <f>$F14*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N14" s="67">
         <f>$F14*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O14" s="67">
         <f>$F14*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P14" s="67">
         <f>$F14*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R14" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S14" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T14" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U14" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.35">
@@ -4612,19 +4612,19 @@
       </c>
       <c r="M15" s="67">
         <f>$F15*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N15" s="67">
         <f>$F15*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O15" s="67">
         <f>$F15*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P15" s="67">
         <f>$F15*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R15" s="67">
         <f t="shared" si="2"/>
@@ -4678,19 +4678,19 @@
       </c>
       <c r="M16" s="67">
         <f>$F16*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N16" s="67">
         <f>$F16*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O16" s="67">
         <f>$F16*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P16" s="67">
         <f>$F16*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R16" s="67">
         <f t="shared" si="2"/>
@@ -4744,35 +4744,35 @@
       </c>
       <c r="M17" s="67">
         <f>$F17*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N17" s="67">
         <f>$F17*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O17" s="67">
         <f>$F17*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P17" s="67">
         <f>$F17*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R17" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S17" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T17" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U17" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.35">
@@ -4810,19 +4810,19 @@
       </c>
       <c r="M18" s="67">
         <f>$F18*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N18" s="67">
         <f>$F18*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O18" s="67">
         <f>$F18*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P18" s="67">
         <f>$F18*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R18" s="67">
         <f t="shared" si="2"/>
@@ -4876,19 +4876,19 @@
       </c>
       <c r="M19" s="67">
         <f>$F19*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N19" s="67">
         <f>$F19*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O19" s="67">
         <f>$F19*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P19" s="67">
         <f>$F19*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R19" s="67">
         <f t="shared" si="2"/>
@@ -4942,35 +4942,35 @@
       </c>
       <c r="M20" s="67">
         <f>$F20*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N20" s="67">
         <f>$F20*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O20" s="67">
         <f>$F20*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P20" s="67">
         <f>$F20*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R20" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S20" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T20" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U20" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.35">
@@ -5008,19 +5008,19 @@
       </c>
       <c r="M21" s="67">
         <f>$F21*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N21" s="67">
         <f>$F21*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O21" s="67">
         <f>$F21*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P21" s="67">
         <f>$F21*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R21" s="67">
         <f t="shared" si="2"/>
@@ -5074,19 +5074,19 @@
       </c>
       <c r="M22" s="67">
         <f>$F22*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N22" s="67">
         <f>$F22*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O22" s="67">
         <f>$F22*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P22" s="67">
         <f>$F22*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R22" s="67">
         <f t="shared" si="2"/>
@@ -5140,35 +5140,35 @@
       </c>
       <c r="M23" s="67">
         <f>$F23*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N23" s="67">
         <f>$F23*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O23" s="67">
         <f>$F23*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P23" s="67">
         <f>$F23*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R23" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S23" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T23" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U23" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.35">
@@ -5206,19 +5206,19 @@
       </c>
       <c r="M24" s="67">
         <f>$F24*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N24" s="67">
         <f>$F24*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O24" s="67">
         <f>$F24*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P24" s="67">
         <f>$F24*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R24" s="67">
         <f t="shared" si="2"/>
@@ -5272,19 +5272,19 @@
       </c>
       <c r="M25" s="67">
         <f>$F25*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N25" s="67">
         <f>$F25*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O25" s="67">
         <f>$F25*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P25" s="67">
         <f>$F25*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R25" s="67">
         <f t="shared" si="2"/>
@@ -5338,35 +5338,35 @@
       </c>
       <c r="M26" s="67">
         <f>$F26*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N26" s="67">
         <f>$F26*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O26" s="67">
         <f>$F26*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P26" s="67">
         <f>$F26*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R26" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S26" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T26" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U26" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.35">
@@ -5404,19 +5404,19 @@
       </c>
       <c r="M27" s="67">
         <f>$F27*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N27" s="67">
         <f>$F27*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O27" s="67">
         <f>$F27*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P27" s="67">
         <f>$F27*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R27" s="67">
         <f t="shared" si="2"/>
@@ -5470,19 +5470,19 @@
       </c>
       <c r="M28" s="67">
         <f>$F28*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N28" s="67">
         <f>$F28*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O28" s="67">
         <f>$F28*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P28" s="67">
         <f>$F28*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R28" s="67">
         <f t="shared" si="2"/>
@@ -5536,35 +5536,35 @@
       </c>
       <c r="M29" s="67">
         <f>$F29*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N29" s="67">
         <f>$F29*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O29" s="67">
         <f>$F29*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P29" s="67">
         <f>$F29*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R29" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S29" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T29" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U29" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.35">
@@ -5602,19 +5602,19 @@
       </c>
       <c r="M30" s="67">
         <f>$F30*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N30" s="67">
         <f>$F30*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O30" s="67">
         <f>$F30*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P30" s="67">
         <f>$F30*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R30" s="67">
         <f t="shared" si="2"/>
@@ -5668,19 +5668,19 @@
       </c>
       <c r="M31" s="67">
         <f>$F31*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N31" s="67">
         <f>$F31*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O31" s="67">
         <f>$F31*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P31" s="67">
         <f>$F31*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R31" s="67">
         <f t="shared" si="2"/>
@@ -5734,35 +5734,35 @@
       </c>
       <c r="M32" s="67">
         <f>$F32*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N32" s="67">
         <f>$F32*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O32" s="67">
         <f>$F32*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P32" s="67">
         <f>$F32*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R32" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S32" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T32" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U32" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.35">
@@ -5800,19 +5800,19 @@
       </c>
       <c r="M33" s="67">
         <f>$F33*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N33" s="67">
         <f>$F33*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O33" s="67">
         <f>$F33*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P33" s="67">
         <f>$F33*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R33" s="67">
         <f t="shared" si="2"/>
@@ -5866,19 +5866,19 @@
       </c>
       <c r="M34" s="67">
         <f>$F34*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N34" s="67">
         <f>$F34*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O34" s="67">
         <f>$F34*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P34" s="67">
         <f>$F34*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R34" s="67">
         <f t="shared" si="2"/>
@@ -5932,35 +5932,35 @@
       </c>
       <c r="M35" s="67">
         <f>$F35*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N35" s="67">
         <f>$F35*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O35" s="67">
         <f>$F35*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P35" s="67">
         <f>$F35*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R35" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S35" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T35" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U35" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.35">
@@ -5998,19 +5998,19 @@
       </c>
       <c r="M36" s="67">
         <f>$F36*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N36" s="67">
         <f>$F36*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O36" s="67">
         <f>$F36*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P36" s="67">
         <f>$F36*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R36" s="67">
         <f t="shared" si="2"/>
@@ -6064,19 +6064,19 @@
       </c>
       <c r="M37" s="67">
         <f>$F37*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N37" s="67">
         <f>$F37*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O37" s="67">
         <f>$F37*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P37" s="67">
         <f>$F37*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R37" s="67">
         <f t="shared" si="2"/>
@@ -6130,35 +6130,35 @@
       </c>
       <c r="M38" s="67">
         <f>$F38*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N38" s="67">
         <f>$F38*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O38" s="67">
         <f>$F38*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P38" s="67">
         <f>$F38*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R38" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S38" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T38" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U38" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.35">
@@ -6196,19 +6196,19 @@
       </c>
       <c r="M39" s="67">
         <f>$F39*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N39" s="67">
         <f>$F39*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O39" s="67">
         <f>$F39*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P39" s="67">
         <f>$F39*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R39" s="67">
         <f t="shared" si="2"/>
@@ -6262,19 +6262,19 @@
       </c>
       <c r="M40" s="67">
         <f>$F40*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N40" s="67">
         <f>$F40*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O40" s="67">
         <f>$F40*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P40" s="67">
         <f>$F40*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R40" s="67">
         <f t="shared" si="2"/>
@@ -6328,35 +6328,35 @@
       </c>
       <c r="M41" s="67">
         <f>$F41*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N41" s="67">
         <f>$F41*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O41" s="67">
         <f>$F41*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P41" s="67">
         <f>$F41*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R41" s="67">
         <f t="shared" si="2"/>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S41" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T41" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U41" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.35">
@@ -6394,19 +6394,19 @@
       </c>
       <c r="M42" s="67">
         <f>$F42*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N42" s="67">
         <f>$F42*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O42" s="67">
         <f>$F42*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P42" s="67">
         <f>$F42*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R42" s="67">
         <f t="shared" si="2"/>
@@ -6460,19 +6460,19 @@
       </c>
       <c r="M43" s="67">
         <f>$F43*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N43" s="67">
         <f>$F43*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O43" s="67">
         <f>$F43*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P43" s="67">
         <f>$F43*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R43" s="67">
         <f t="shared" si="2"/>
@@ -6526,35 +6526,35 @@
       </c>
       <c r="M44" s="67">
         <f>$F44*Outputs_Internal!$D$50/12</f>
-        <v>18327.916666666668</v>
+        <v>17062.916666666668</v>
       </c>
       <c r="N44" s="67">
         <f>$F44*Outputs_Internal!J$50/12</f>
-        <v>6900.5378782396847</v>
+        <v>6644.6002418339631</v>
       </c>
       <c r="O44" s="67">
         <f>$F44*Outputs_Internal!K$50/12</f>
-        <v>9114.4234234234227</v>
+        <v>8942.3113893858081</v>
       </c>
       <c r="P44" s="67">
         <f>$F44*Outputs_Internal!L$50/12</f>
-        <v>2312.9553650035582</v>
+        <v>1476.0050354468967</v>
       </c>
       <c r="R44" s="67">
         <f>IF(MOD(MONTH($B44),3)=0,SUM(H42:H44,M42:M44),0)</f>
-        <v>54983.75</v>
+        <v>51188.75</v>
       </c>
       <c r="S44" s="67">
         <f t="shared" si="3"/>
-        <v>20701.613634719055</v>
+        <v>19933.800725501889</v>
       </c>
       <c r="T44" s="67">
         <f t="shared" si="4"/>
-        <v>27343.270270270266</v>
+        <v>26826.934168157422</v>
       </c>
       <c r="U44" s="67">
         <f t="shared" si="5"/>
-        <v>6938.8660950106751</v>
+        <v>4428.0151063406902</v>
       </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.35">
@@ -10153,7 +10153,7 @@
       </c>
       <c r="E15" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E13="Y",Inputs!E$19="Y"), Prices!$C14, 0)</f>
-        <v>7200</v>
+        <v>0</v>
       </c>
       <c r="F15" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!F13="Y",Inputs!F$19="Y"), Prices!$C14, 0)</f>
@@ -10178,7 +10178,7 @@
       </c>
       <c r="E16" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E14="Y",Inputs!E$19="Y"), Prices!$C15, 0)</f>
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="F16" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!F14="Y",Inputs!F$19="Y"), Prices!$C15, 0)</f>
@@ -10428,7 +10428,7 @@
       </c>
       <c r="E28" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$6 = 0), 0, IF(OR(Inputs!E13="Y",Inputs!E$19="Y"),PRODUCT(E$6, Prices!$D14),0))</f>
-        <v>3500.0000000000005</v>
+        <v>0</v>
       </c>
       <c r="F28" s="18">
         <f>IF(OR(Inputs!F$4="Y", F$6 = 0), 0, IF(OR(Inputs!F13="Y",Inputs!F$19="Y"),PRODUCT(F$6, Prices!$D14),0))</f>
@@ -10453,7 +10453,7 @@
       </c>
       <c r="E29" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$6 = 0), 0, IF(OR(Inputs!E14="Y",Inputs!E$19="Y"),PRODUCT(E$6, Prices!$D15),0))</f>
-        <v>3500.0000000000005</v>
+        <v>0</v>
       </c>
       <c r="F29" s="18">
         <f>IF(OR(Inputs!F$4="Y", F$6 = 0), 0, IF(OR(Inputs!F14="Y",Inputs!F$19="Y"),PRODUCT(F$6, Prices!$D15),0))</f>
@@ -10610,7 +10610,7 @@
       </c>
       <c r="E37" s="18">
         <f>IF(AND(Inputs!E9="Y",Inputs!E$19="N"),Prices!$C10,0)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="F37" s="18">
         <f>IF(AND(Inputs!F9="Y",Inputs!F$19="N"),Prices!$C10,0)</f>
@@ -10635,7 +10635,7 @@
       </c>
       <c r="E38" s="18">
         <f>IF(AND(Inputs!E10="Y",Inputs!E$19="N"),Prices!$C11,0)</f>
-        <v>0</v>
+        <v>4800</v>
       </c>
       <c r="F38" s="18">
         <f>IF(AND(Inputs!F10="Y",Inputs!F$19="N"),Prices!$C11,0)</f>
@@ -10660,7 +10660,7 @@
       </c>
       <c r="E39" s="18">
         <f>IF(AND(Inputs!E11="Y",Inputs!E$19="N"),Prices!$C12,0)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="F39" s="18">
         <f>IF(AND(Inputs!F11="Y",Inputs!F$19="N"),Prices!$C12,0)</f>
@@ -10685,7 +10685,7 @@
       </c>
       <c r="E40" s="18">
         <f>IF(AND(Inputs!E12="Y",Inputs!E$19="N"),Prices!$C13,0)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="F40" s="18">
         <f>IF(AND(Inputs!F12="Y",Inputs!F$19="N"),Prices!$C13,0)</f>
@@ -10885,7 +10885,7 @@
       </c>
       <c r="E50" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$6 = 0), 0, IF(AND(Inputs!E9="Y",Inputs!E$19="N"),PRODUCT(E$6, Prices!$D10),0))</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F50" s="18">
         <f>IF(OR(Inputs!F$4="Y", F$6 = 0), 0, IF(AND(Inputs!F9="Y",Inputs!F$19="N"),PRODUCT(F$6, Prices!$D10),0))</f>
@@ -10910,7 +10910,7 @@
       </c>
       <c r="E51" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$6 = 0), 0, IF(AND(Inputs!E10="Y",Inputs!E$19="N"),PRODUCT(E$6, Prices!$D11),0))</f>
-        <v>0</v>
+        <v>3500.0000000000005</v>
       </c>
       <c r="F51" s="18">
         <f>IF(OR(Inputs!F$4="Y", F$6 = 0), 0, IF(AND(Inputs!F10="Y",Inputs!F$19="N"),PRODUCT(F$6, Prices!$D11),0))</f>
@@ -10935,7 +10935,7 @@
       </c>
       <c r="E52" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$6 = 0), 0, IF(AND(Inputs!E11="Y",Inputs!E$19="N"),PRODUCT(E$6, Prices!$D12),0))</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F52" s="18">
         <f>IF(OR(Inputs!F$4="Y", F$6 = 0), 0, IF(AND(Inputs!F11="Y",Inputs!F$19="N"),PRODUCT(F$6, Prices!$D12),0))</f>
@@ -10960,7 +10960,7 @@
       </c>
       <c r="E53" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$6 = 0), 0, IF(AND(Inputs!E12="Y",Inputs!E$19="N"),PRODUCT(E$6, Prices!$D13),0))</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F53" s="18">
         <f>IF(OR(Inputs!F$4="Y", F$6 = 0), 0, IF(AND(Inputs!F12="Y",Inputs!F$19="N"),PRODUCT(F$6, Prices!$D13),0))</f>
@@ -11105,23 +11105,23 @@
         <v>18</v>
       </c>
       <c r="D61" s="18">
-        <f>IF(Inputs!$D$19 = "Y", 0, IF(Inputs!D18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!D$19 = "Y", 0, IF(Inputs!D18="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="E61" s="18">
-        <f>IF(Inputs!$D$19 = "Y", 0, IF(Inputs!E18="Y", Prices!$C20, 0))</f>
-        <v>0</v>
+        <f>IF(Inputs!E$19 = "Y", 0, IF(Inputs!E18="Y", Prices!$C20, 0))</f>
+        <v>10200</v>
       </c>
       <c r="F61" s="18">
-        <f>IF(Inputs!$D$19 = "Y", 0, IF(Inputs!F18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!F$19 = "Y", 0, IF(Inputs!F18="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="G61" s="18">
-        <f>IF(Inputs!$D$19 = "Y", 0, IF(Inputs!G18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!G$19 = "Y", 0, IF(Inputs!G18="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="H61" s="18">
-        <f>IF(Inputs!$D$19 = "Y", 0, IF(Inputs!H18="Y", Prices!$C20, 0))</f>
+        <f>IF(Inputs!H$19 = "Y", 0, IF(Inputs!H18="Y", Prices!$C20, 0))</f>
         <v>0</v>
       </c>
       <c r="K61" s="21">
@@ -11130,7 +11130,7 @@
       </c>
       <c r="L61" s="21">
         <f>IF(COUNTIF(E$61:E$64,"")&gt;2,"",IFERROR(RANK(E61,E$61:E$64),4))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M61" s="21">
         <f t="shared" ref="M61:M64" si="1">IF(COUNTIF(F$61:F$64,"")&gt;2,"",IFERROR(RANK(F61,F$61:F$64),4))</f>
@@ -11155,7 +11155,7 @@
       </c>
       <c r="E62" s="18">
         <f>IF(Inputs!E19="Y", Prices!$C21, 0)</f>
-        <v>39600</v>
+        <v>0</v>
       </c>
       <c r="F62" s="18">
         <f>IF(Inputs!F19="Y", Prices!$C21, 0)</f>
@@ -11175,7 +11175,7 @@
       </c>
       <c r="L62" s="21">
         <f t="shared" ref="L62:L64" si="4">IF(COUNTIF(E$61:E$64,"")&gt;2,"",IFERROR(RANK(E62,E$61:E$64),4))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M62" s="21">
         <f t="shared" si="1"/>
@@ -11335,7 +11335,7 @@
       </c>
       <c r="E68" s="18">
         <f>IF(Inputs!E$4="Y", 0, IF(E$6 = "", 0, IF(Inputs!E19 = "Y", E$6*Prices!$D21, 0)))</f>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="F68" s="18">
         <f>IF(Inputs!F$4="Y", 0, IF(F$6 = "", 0, IF(Inputs!F19 = "Y", F$6*Prices!$D21, 0)))</f>
@@ -11422,7 +11422,7 @@
       </c>
       <c r="E73" s="18">
         <f t="shared" ref="E73:H73" si="9">E61</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="F73" s="18">
         <f t="shared" si="9"/>
@@ -11447,7 +11447,7 @@
       </c>
       <c r="E74" s="18">
         <f t="shared" ref="E74:H74" si="10">IF(E62=0,0,E62-SUM(E11:E16))</f>
-        <v>16800</v>
+        <v>0</v>
       </c>
       <c r="F74" s="18">
         <f>IF(F62=0,0,F62-SUM(F11:F16))</f>
@@ -11567,7 +11567,7 @@
       </c>
       <c r="E80" s="18">
         <f t="shared" ref="E80:H80" si="17">IF(E68=0,0,E68-SUM(E24:E29))</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F80" s="18">
         <f t="shared" si="17"/>
@@ -11697,7 +11697,7 @@
       </c>
       <c r="E88" s="7">
         <f t="shared" ref="E88:H88" si="20">SUM(E35:E45, E48:E58, E61:E64, E67:E70, E85:E86)</f>
-        <v>120700</v>
+        <v>93100</v>
       </c>
       <c r="F88" s="7">
         <f t="shared" si="20"/>
@@ -11725,11 +11725,11 @@
       </c>
       <c r="E90" s="1">
         <f t="shared" ref="E90:H90" si="21">IF(E98=1, 0, IF(E98=2, $E$101, IF(E98=3, $E$102, IF(E98=4, $E$103, IF(E98=5, $E$104, "")))))</f>
-        <v>0</v>
+        <v>-41895</v>
       </c>
       <c r="F90" s="1">
         <f t="shared" si="21"/>
-        <v>-54315</v>
+        <v>0</v>
       </c>
       <c r="G90" s="1">
         <f t="shared" si="21"/>
@@ -11750,11 +11750,11 @@
       </c>
       <c r="E92" s="7">
         <f>SUM(E88, E90)</f>
-        <v>120700</v>
+        <v>51205</v>
       </c>
       <c r="F92" s="7">
         <f>SUM(F88, F90)</f>
-        <v>66385</v>
+        <v>120700</v>
       </c>
       <c r="G92" s="7">
         <f>SUM(G88, G90)</f>
@@ -11776,7 +11776,7 @@
       </c>
       <c r="E95" s="21">
         <f t="shared" ref="E95:H95" si="22">IFERROR(_xlfn.RANK.EQ(E88,$D$88:$H$88),5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F95" s="21">
         <f t="shared" si="22"/>
@@ -11817,7 +11817,7 @@
       </c>
       <c r="E97" s="21">
         <f t="shared" ref="E97:H97" si="23">SUM(E95:E96)</f>
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F97" s="21">
         <f t="shared" si="23"/>
@@ -11840,11 +11840,11 @@
       </c>
       <c r="E98" s="21">
         <f t="shared" ref="E98:H98" si="24">_xlfn.RANK.EQ(E97, $D$97:$H$97, 5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F98" s="21">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G98" s="21">
         <f t="shared" si="24"/>
@@ -11871,7 +11871,7 @@
       </c>
       <c r="E101" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(2, $D$98:$H$98, 0))*Prices!$I$10*-1</f>
-        <v>-54315</v>
+        <v>-41895</v>
       </c>
     </row>
     <row r="102" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add preliminary revenue percentages
Do this to get a start on the revenue split discussion. Seeded with
McLaren as the example client.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="101">
   <si>
     <t>One-Time Fees:</t>
   </si>
@@ -1005,7 +1005,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1057,9 @@
       <c r="B4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="56" t="s">
+        <v>4</v>
+      </c>
       <c r="E4" s="56"/>
       <c r="F4" s="56"/>
       <c r="G4" s="56"/>
@@ -1070,7 +1072,9 @@
       <c r="B5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E5" s="56"/>
       <c r="F5" s="56"/>
       <c r="G5" s="56"/>
@@ -1083,7 +1087,9 @@
       <c r="B6" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E6" s="56"/>
       <c r="F6" s="56"/>
       <c r="G6" s="56"/>
@@ -1093,7 +1099,9 @@
       <c r="B7" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="56">
+        <v>50000</v>
+      </c>
       <c r="E7" s="56"/>
       <c r="F7" s="56"/>
       <c r="G7" s="56"/>
@@ -1103,7 +1111,9 @@
       <c r="B8" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="56" t="s">
+        <v>4</v>
+      </c>
       <c r="E8" s="56"/>
       <c r="F8" s="56"/>
       <c r="G8" s="56"/>
@@ -1113,7 +1123,9 @@
       <c r="B9" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="56"/>
+      <c r="D9" s="56" t="s">
+        <v>4</v>
+      </c>
       <c r="E9" s="56"/>
       <c r="F9" s="56"/>
       <c r="G9" s="56"/>
@@ -1123,7 +1135,9 @@
       <c r="B10" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="56"/>
+      <c r="D10" s="56" t="s">
+        <v>4</v>
+      </c>
       <c r="E10" s="56"/>
       <c r="F10" s="56"/>
       <c r="G10" s="56"/>
@@ -1133,7 +1147,9 @@
       <c r="B11" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="56"/>
+      <c r="D11" s="56" t="s">
+        <v>4</v>
+      </c>
       <c r="E11" s="56"/>
       <c r="F11" s="56"/>
       <c r="G11" s="56"/>
@@ -1143,7 +1159,9 @@
       <c r="B12" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="56"/>
+      <c r="D12" s="56" t="s">
+        <v>4</v>
+      </c>
       <c r="E12" s="56"/>
       <c r="F12" s="56"/>
       <c r="G12" s="56"/>
@@ -1153,7 +1171,9 @@
       <c r="B13" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="56"/>
+      <c r="D13" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E13" s="56"/>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
@@ -1163,7 +1183,9 @@
       <c r="B14" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="56"/>
+      <c r="D14" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E14" s="56"/>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
@@ -1173,7 +1195,9 @@
       <c r="B15" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E15" s="56"/>
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
@@ -1183,7 +1207,9 @@
       <c r="B16" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="56"/>
+      <c r="D16" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E16" s="56"/>
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
@@ -1193,7 +1219,9 @@
       <c r="B17" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="56"/>
+      <c r="D17" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E17" s="56"/>
       <c r="F17" s="56"/>
       <c r="G17" s="56"/>
@@ -1203,7 +1231,9 @@
       <c r="B18" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="56"/>
+      <c r="D18" s="56" t="s">
+        <v>4</v>
+      </c>
       <c r="E18" s="56"/>
       <c r="F18" s="56"/>
       <c r="G18" s="56"/>
@@ -1213,7 +1243,9 @@
       <c r="B19" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="56"/>
+      <c r="D19" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E19" s="56"/>
       <c r="F19" s="56"/>
       <c r="G19" s="56"/>
@@ -1223,7 +1255,9 @@
       <c r="B20" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="56"/>
+      <c r="D20" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="E20" s="56"/>
       <c r="F20" s="56"/>
       <c r="G20" s="56"/>
@@ -1234,7 +1268,9 @@
         <v>21</v>
       </c>
       <c r="C21" s="71"/>
-      <c r="D21" s="58"/>
+      <c r="D21" s="58" t="s">
+        <v>45</v>
+      </c>
       <c r="E21" s="58"/>
       <c r="F21" s="58"/>
       <c r="G21" s="58"/>
@@ -1309,7 +1345,7 @@
       </c>
       <c r="D4" s="1">
         <f>MAX(Calcs!D4, 0)</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="1">
         <f>MAX(Calcs!E4, 0)</f>
@@ -1360,7 +1396,7 @@
       </c>
       <c r="D7" s="16">
         <f>SUM(Calcs!D35, Calcs!D48)</f>
-        <v>0</v>
+        <v>18000</v>
       </c>
       <c r="E7" s="16">
         <f>SUM(Calcs!E35, Calcs!E48)</f>
@@ -1396,7 +1432,7 @@
       </c>
       <c r="D8" s="16">
         <f>SUM(Calcs!D36, Calcs!D49)</f>
-        <v>0</v>
+        <v>8100</v>
       </c>
       <c r="E8" s="16">
         <f>SUM(Calcs!E36, Calcs!E49)</f>
@@ -1432,7 +1468,7 @@
       </c>
       <c r="D9" s="18">
         <f>SUM(Calcs!D37, Calcs!D50)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="E9" s="18">
         <f>SUM(Calcs!E37, Calcs!E50)</f>
@@ -1468,7 +1504,7 @@
       </c>
       <c r="D10" s="18">
         <f>SUM(Calcs!D38, Calcs!D51)</f>
-        <v>0</v>
+        <v>4800</v>
       </c>
       <c r="E10" s="18">
         <f>SUM(Calcs!E38, Calcs!E51)</f>
@@ -1504,7 +1540,7 @@
       </c>
       <c r="D11" s="18">
         <f>SUM(Calcs!D39, Calcs!D52)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="E11" s="18">
         <f>SUM(Calcs!E39, Calcs!E52)</f>
@@ -1539,7 +1575,7 @@
       </c>
       <c r="D12" s="18">
         <f>SUM(Calcs!D40, Calcs!D53)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="E12" s="18">
         <f>SUM(Calcs!E40, Calcs!E53)</f>
@@ -1754,7 +1790,7 @@
       </c>
       <c r="D20" s="1">
         <f>SUM(Calcs!D61, Calcs!D67)</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="E20" s="1">
         <f>SUM(Calcs!E61, Calcs!E67)</f>
@@ -1969,7 +2005,7 @@
       </c>
       <c r="D29" s="7">
         <f>SUM(D7:D17, D20:D23, D26:D27)</f>
-        <v>0</v>
+        <v>47100</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" ref="E29:H29" si="0">SUM(E7:E17, E20:E23, E26:E27)</f>
@@ -2041,7 +2077,7 @@
       </c>
       <c r="D34" s="7">
         <f>(D29/12*Inputs!$C$2+D4)*$C$32</f>
-        <v>0</v>
+        <v>146300</v>
       </c>
       <c r="E34" s="7">
         <f>(E29/12*Inputs!$C$2+E4)*$C$32</f>
@@ -2090,13 +2126,13 @@
     <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C38" s="7">
         <f>SUM(Outputs_Timeline!R:R)</f>
-        <v>0</v>
+        <v>146300</v>
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" s="53">
         <f>SUM(D34:H34)</f>
-        <v>0</v>
+        <v>146300</v>
       </c>
       <c r="D39" s="1"/>
       <c r="G39" s="1"/>
@@ -2129,7 +2165,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,14 +2225,14 @@
       </c>
       <c r="D4" s="1">
         <f>SUM(Outputs_External!D4:'Outputs_External'!H4)</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="10">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G4" s="10">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="H4" s="52">
         <f>1-SUM(F4:G4)</f>
@@ -2204,11 +2240,11 @@
       </c>
       <c r="J4" s="12">
         <f>F4*$D4</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="K4" s="12">
         <f>G4*$D4</f>
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="L4" s="12">
         <f>H4*$D4</f>
@@ -2240,14 +2276,14 @@
       </c>
       <c r="D7" s="16">
         <f>SUM(Calcs!D9:H9)</f>
-        <v>0</v>
+        <v>18000</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="32">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="G7" s="32">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="H7" s="35">
         <f t="shared" ref="H7:H17" si="0">1-SUM(F7:G7)</f>
@@ -2255,11 +2291,11 @@
       </c>
       <c r="J7" s="16">
         <f>F7*$D7</f>
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="K7" s="16">
         <f>G7*$D7</f>
-        <v>0</v>
+        <v>12600</v>
       </c>
       <c r="L7" s="16">
         <f t="shared" ref="L7:L17" si="1">H7*$D7</f>
@@ -2272,14 +2308,14 @@
       </c>
       <c r="D8" s="16">
         <f>SUM(Calcs!D10:H10)</f>
-        <v>0</v>
+        <v>8100</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="32">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G8" s="32">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="H8" s="35">
         <f t="shared" si="0"/>
@@ -2287,11 +2323,11 @@
       </c>
       <c r="J8" s="16">
         <f t="shared" ref="J8:J17" si="2">F8*$D8</f>
-        <v>0</v>
+        <v>1620</v>
       </c>
       <c r="K8" s="16">
         <f t="shared" ref="K8:K16" si="3">G8*$D8</f>
-        <v>0</v>
+        <v>6480</v>
       </c>
       <c r="L8" s="16">
         <f t="shared" si="1"/>
@@ -2304,14 +2340,14 @@
       </c>
       <c r="D9" s="18">
         <f>SUM(Calcs!D11:H11)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="33">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G9" s="33">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="H9" s="37">
         <f t="shared" si="0"/>
@@ -2319,11 +2355,11 @@
       </c>
       <c r="J9" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="K9" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1080</v>
       </c>
       <c r="L9" s="18">
         <f t="shared" si="1"/>
@@ -2336,14 +2372,14 @@
       </c>
       <c r="D10" s="18">
         <f>SUM(Calcs!D12:H12)</f>
-        <v>0</v>
+        <v>4800</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="33">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G10" s="33">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="H10" s="37">
         <f t="shared" si="0"/>
@@ -2351,11 +2387,11 @@
       </c>
       <c r="J10" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="K10" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4320</v>
       </c>
       <c r="L10" s="18">
         <f t="shared" si="1"/>
@@ -2368,13 +2404,13 @@
       </c>
       <c r="D11" s="18">
         <f>SUM(Calcs!D13:H13)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="F11" s="33">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="G11" s="33">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H11" s="37">
         <f t="shared" si="0"/>
@@ -2382,11 +2418,11 @@
       </c>
       <c r="J11" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2160</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="L11" s="18">
         <f t="shared" si="1"/>
@@ -2399,13 +2435,13 @@
       </c>
       <c r="D12" s="18">
         <f>SUM(Calcs!D14:H14)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="F12" s="33">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G12" s="33">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="H12" s="37">
         <f t="shared" si="0"/>
@@ -2413,11 +2449,11 @@
       </c>
       <c r="J12" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="K12" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2160</v>
       </c>
       <c r="L12" s="18">
         <f t="shared" si="1"/>
@@ -2495,10 +2531,10 @@
         <v>0</v>
       </c>
       <c r="F15" s="34">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="G15" s="34">
-        <v>0.6</v>
+        <v>0.98</v>
       </c>
       <c r="H15" s="38">
         <f t="shared" si="0"/>
@@ -2526,10 +2562,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="34">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="G16" s="34">
-        <v>0.6</v>
+        <v>0.98</v>
       </c>
       <c r="H16" s="38">
         <f t="shared" si="0"/>
@@ -2557,10 +2593,10 @@
         <v>0</v>
       </c>
       <c r="F17" s="34">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="G17" s="34">
-        <v>0.6</v>
+        <v>0.98</v>
       </c>
       <c r="H17" s="38">
         <f t="shared" si="0"/>
@@ -2628,11 +2664,11 @@
       <c r="E22" s="3"/>
       <c r="F22" s="35">
         <f>(1-G22)*F7/SUM(F7,H7)</f>
-        <v>0.30000000000000004</v>
+        <v>0.20000000000000007</v>
       </c>
       <c r="G22" s="35">
         <f t="shared" ref="G22:G32" si="4">MIN(1,G7+$H$19)</f>
-        <v>0.7</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="H22" s="35">
         <f>(1-G22)*H7/SUM(F7,H7)</f>
@@ -2662,11 +2698,11 @@
       <c r="E23" s="3"/>
       <c r="F23" s="36">
         <f t="shared" ref="F23:F32" si="7">(1-G23)*F8/SUM(F8,H8)</f>
-        <v>0.30000000000000004</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="G23" s="36">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="H23" s="36">
         <f t="shared" ref="H23:H32" si="8">(1-G23)*H8/SUM(F8,H8)</f>
@@ -2696,11 +2732,11 @@
       <c r="E24" s="3"/>
       <c r="F24" s="37">
         <f t="shared" si="7"/>
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G24" s="37">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H24" s="37">
         <f t="shared" si="8"/>
@@ -2730,11 +2766,11 @@
       <c r="E25" s="3"/>
       <c r="F25" s="37">
         <f t="shared" si="7"/>
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G25" s="37">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H25" s="37">
         <f t="shared" si="8"/>
@@ -2763,11 +2799,11 @@
       </c>
       <c r="F26" s="37">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G26" s="37">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="H26" s="37">
         <f t="shared" si="8"/>
@@ -2796,11 +2832,11 @@
       </c>
       <c r="F27" s="37">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G27" s="37">
         <f t="shared" si="4"/>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="H27" s="37">
         <f t="shared" si="8"/>
@@ -2895,11 +2931,11 @@
       </c>
       <c r="F30" s="38">
         <f t="shared" si="7"/>
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G30" s="38">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H30" s="38">
         <f t="shared" si="8"/>
@@ -2928,11 +2964,11 @@
       </c>
       <c r="F31" s="38">
         <f t="shared" si="7"/>
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G31" s="38">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H31" s="38">
         <f t="shared" si="8"/>
@@ -2961,11 +2997,11 @@
       </c>
       <c r="F32" s="36">
         <f t="shared" si="7"/>
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G32" s="36">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H32" s="36">
         <f t="shared" si="8"/>
@@ -3009,28 +3045,28 @@
       </c>
       <c r="D35" s="18">
         <f>SUM(Calcs!D73:H73)</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="F35" s="33">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G35" s="33">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H35" s="37">
-        <f t="shared" ref="H35:H38" si="10">1-SUM(F35:G35)</f>
+        <f>1-SUM(F35:G35)</f>
         <v>0</v>
       </c>
       <c r="J35" s="18">
         <f>F35*$D35</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="K35" s="18">
-        <f t="shared" ref="J35:L38" si="11">G35*$D35</f>
+        <f t="shared" ref="J35:L38" si="10">G35*$D35</f>
         <v>0</v>
       </c>
       <c r="L35" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -3043,25 +3079,25 @@
         <v>0</v>
       </c>
       <c r="F36" s="33">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G36" s="33">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H36" s="37">
+        <f>1-SUM(F36:G36)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="18">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J36" s="18">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
       <c r="K36" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L36" s="18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -3074,25 +3110,25 @@
         <v>0</v>
       </c>
       <c r="F37" s="34">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="G37" s="34">
-        <v>0.6</v>
+        <v>0.98</v>
       </c>
       <c r="H37" s="38">
+        <f t="shared" ref="H35:H38" si="11">1-SUM(F37:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="20">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J37" s="20">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
       <c r="K37" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L37" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -3105,25 +3141,25 @@
         <v>0</v>
       </c>
       <c r="F38" s="34">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="G38" s="34">
-        <v>0.6</v>
+        <v>0.98</v>
       </c>
       <c r="H38" s="38">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="20">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J38" s="20">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
       <c r="K38" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L38" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -3153,11 +3189,11 @@
       </c>
       <c r="F41" s="50">
         <f>IFERROR((1-G41)*F35/SUM(F35,H35),0)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G41" s="50">
         <f>MIN(1,G35+$H$19)</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H41" s="50">
         <f>IFERROR((1-G41)*H35/SUM(F35,H35),0)</f>
@@ -3186,11 +3222,11 @@
       </c>
       <c r="F42" s="30">
         <f>IFERROR((1-G42)*F36/SUM(F36,H36),0)</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G42" s="30">
         <f t="shared" ref="G42:G44" si="14">MIN(1,G36+$H$19)</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H42" s="30">
         <f>IFERROR((1-G42)*H36/SUM(F36,H36),0)</f>
@@ -3219,11 +3255,11 @@
       </c>
       <c r="F43" s="31">
         <f>IFERROR((1-G43)*F37/SUM(F37,H37),0)</f>
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G43" s="31">
         <f t="shared" si="14"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H43" s="31">
         <f>IFERROR((1-G43)*H37/SUM(F37,H37),0)</f>
@@ -3252,11 +3288,11 @@
       </c>
       <c r="F44" s="31">
         <f>IFERROR((1-G44)*F38/SUM(F38,H38),0)</f>
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="G44" s="31">
         <f t="shared" si="14"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H44" s="31">
         <f>IFERROR((1-G44)*H38/SUM(F38,H38),0)</f>
@@ -3298,7 +3334,7 @@
       </c>
       <c r="F47" s="8">
         <f>IFERROR(SUM(J58:J61)/SUM($J$58:$L$61), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="8">
         <f>IFERROR(SUM(K58:K61)/SUM($J$58:$L$61), 0)</f>
@@ -3331,15 +3367,15 @@
       </c>
       <c r="F48" s="3">
         <f>IFERROR(SUM(J7:J47)/SUM(J7:L47), 0)</f>
-        <v>0</v>
+        <v>0.42929936305732486</v>
       </c>
       <c r="G48" s="3">
         <f>IFERROR(SUM(K7:K47)/SUM(J7:L47), 0)</f>
-        <v>0</v>
+        <v>0.57070063694267514</v>
       </c>
       <c r="H48" s="3">
         <f>1-F48-G48</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="12">
         <f>F48*$D$48</f>
@@ -3365,15 +3401,15 @@
       </c>
       <c r="D50" s="1">
         <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
-        <v>0</v>
+        <v>47100</v>
       </c>
       <c r="J50" s="12">
         <f>SUM(J47:J48, J35:J38, J7:J17,J22:J32,J41:J44)</f>
-        <v>0</v>
+        <v>20220</v>
       </c>
       <c r="K50" s="12">
         <f t="shared" ref="K50:L50" si="16">SUM(K47:K48, K35:K38, K7:K17,K22:K32,K41:K44)</f>
-        <v>0</v>
+        <v>26880</v>
       </c>
       <c r="L50" s="12">
         <f t="shared" si="16"/>
@@ -3386,7 +3422,7 @@
       </c>
       <c r="D51" s="23">
         <f>SUM(J50:L50)</f>
-        <v>0</v>
+        <v>47100</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
@@ -3403,15 +3439,15 @@
       </c>
       <c r="D53" s="1">
         <f>SUM(Outputs_Timeline!R:R)</f>
-        <v>0</v>
+        <v>146300</v>
       </c>
       <c r="J53" s="12">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>0</v>
+        <v>61160</v>
       </c>
       <c r="K53" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>0</v>
+        <v>85140</v>
       </c>
       <c r="L53" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
@@ -3420,17 +3456,17 @@
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
-      <c r="J54" s="54" t="e">
-        <f>J53/$D$53</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K54" s="54" t="e">
-        <f t="shared" ref="K54:L54" si="17">K53/$D$53</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L54" s="54" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+      <c r="J54" s="54">
+        <f>IFERROR(J53/$D$53, 0)</f>
+        <v>0.41804511278195489</v>
+      </c>
+      <c r="K54" s="54">
+        <f>IFERROR(K53/$D$53, 0)</f>
+        <v>0.58195488721804511</v>
+      </c>
+      <c r="L54" s="54">
+        <f>IFERROR(L53/$D$53, 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
@@ -3460,16 +3496,16 @@
       </c>
       <c r="D58" s="23">
         <f>SUM(Calcs!D61:H61)+SUM(Calcs!D67:H67)</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="E58" s="21"/>
       <c r="F58" s="24">
         <f>F35</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G58" s="24">
         <f>G35</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H58" s="24">
         <f>H35</f>
@@ -3477,15 +3513,15 @@
       </c>
       <c r="I58" s="21"/>
       <c r="J58" s="25">
-        <f t="shared" ref="J58:L61" si="18">F58*$D58</f>
-        <v>0</v>
+        <f t="shared" ref="J58:L61" si="17">F58*$D58</f>
+        <v>10200</v>
       </c>
       <c r="K58" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L58" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -3501,27 +3537,27 @@
       <c r="E59" s="21"/>
       <c r="F59" s="24">
         <f>IFERROR(SUM(J$36,J$9:J$14,J$42,J$24:J$29)/SUM($J$36:$L$36,$J$9:$L$14,$J$42:$L$42,$J$24:$L$29),0)</f>
-        <v>0</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="G59" s="24">
-        <f t="shared" ref="G59:H59" si="19">IFERROR(SUM(K$36,K$9:K$14,K$42,K$24:K$29)/SUM($J$36:$L$36,$J$9:$L$14,$J$42:$L$42,$J$24:$L$29),0)</f>
-        <v>0</v>
+        <f t="shared" ref="G59:H59" si="18">IFERROR(SUM(K$36,K$9:K$14,K$42,K$24:K$29)/SUM($J$36:$L$36,$J$9:$L$14,$J$42:$L$42,$J$24:$L$29),0)</f>
+        <v>0.72222222222222221</v>
       </c>
       <c r="H59" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I59" s="21"/>
       <c r="J59" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K59" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L59" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -3549,15 +3585,15 @@
       </c>
       <c r="I60" s="21"/>
       <c r="J60" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K60" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L60" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -3573,11 +3609,11 @@
       <c r="E61" s="21"/>
       <c r="F61" s="24">
         <f>F38</f>
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="G61" s="24">
         <f>G38</f>
-        <v>0.6</v>
+        <v>0.98</v>
       </c>
       <c r="H61" s="24">
         <f>H38</f>
@@ -3585,15 +3621,15 @@
       </c>
       <c r="I61" s="21"/>
       <c r="J61" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K61" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L61" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4092,15 +4128,15 @@
       </c>
       <c r="H9" s="67">
         <f>IF($B9=Inputs!$C$1,Outputs_Internal!$D$4,0)*$D9</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="I9" s="67">
         <f>IF($B9=Inputs!$C$1,Outputs_Internal!J$4,0)*$D9</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="J9" s="67">
         <f>IF($B9=Inputs!$C$1,Outputs_Internal!K$4,0)*$D9</f>
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="K9" s="67">
         <f>IF($B9=Inputs!$C$1,Outputs_Internal!L$4,0)*$D9</f>
@@ -4108,15 +4144,15 @@
       </c>
       <c r="M9" s="67">
         <f>$F9*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N9" s="67">
         <f>$F9*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O9" s="67">
         <f>$F9*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P9" s="67">
         <f>$F9*Outputs_Internal!L$50/12</f>
@@ -4174,15 +4210,15 @@
       </c>
       <c r="M10" s="67">
         <f>$F10*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N10" s="67">
         <f>$F10*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O10" s="67">
         <f>$F10*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P10" s="67">
         <f>$F10*Outputs_Internal!L$50/12</f>
@@ -4240,15 +4276,15 @@
       </c>
       <c r="M11" s="67">
         <f>$F11*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N11" s="67">
         <f>$F11*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O11" s="67">
         <f>$F11*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P11" s="67">
         <f>$F11*Outputs_Internal!L$50/12</f>
@@ -4256,15 +4292,15 @@
       </c>
       <c r="R11" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16775</v>
       </c>
       <c r="S11" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5555</v>
       </c>
       <c r="T11" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>11220</v>
       </c>
       <c r="U11" s="67">
         <f t="shared" si="5"/>
@@ -4306,15 +4342,15 @@
       </c>
       <c r="M12" s="67">
         <f>$F12*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N12" s="67">
         <f>$F12*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O12" s="67">
         <f>$F12*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P12" s="67">
         <f>$F12*Outputs_Internal!L$50/12</f>
@@ -4372,15 +4408,15 @@
       </c>
       <c r="M13" s="67">
         <f>$F13*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N13" s="67">
         <f>$F13*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O13" s="67">
         <f>$F13*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P13" s="67">
         <f>$F13*Outputs_Internal!L$50/12</f>
@@ -4438,15 +4474,15 @@
       </c>
       <c r="M14" s="67">
         <f>$F14*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N14" s="67">
         <f>$F14*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O14" s="67">
         <f>$F14*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P14" s="67">
         <f>$F14*Outputs_Internal!L$50/12</f>
@@ -4454,15 +4490,15 @@
       </c>
       <c r="R14" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S14" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T14" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U14" s="67">
         <f t="shared" si="5"/>
@@ -4504,15 +4540,15 @@
       </c>
       <c r="M15" s="67">
         <f>$F15*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N15" s="67">
         <f>$F15*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O15" s="67">
         <f>$F15*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P15" s="67">
         <f>$F15*Outputs_Internal!L$50/12</f>
@@ -4570,15 +4606,15 @@
       </c>
       <c r="M16" s="67">
         <f>$F16*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N16" s="67">
         <f>$F16*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O16" s="67">
         <f>$F16*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P16" s="67">
         <f>$F16*Outputs_Internal!L$50/12</f>
@@ -4636,15 +4672,15 @@
       </c>
       <c r="M17" s="67">
         <f>$F17*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N17" s="67">
         <f>$F17*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O17" s="67">
         <f>$F17*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P17" s="67">
         <f>$F17*Outputs_Internal!L$50/12</f>
@@ -4652,15 +4688,15 @@
       </c>
       <c r="R17" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S17" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T17" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U17" s="67">
         <f t="shared" si="5"/>
@@ -4702,15 +4738,15 @@
       </c>
       <c r="M18" s="67">
         <f>$F18*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N18" s="67">
         <f>$F18*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O18" s="67">
         <f>$F18*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P18" s="67">
         <f>$F18*Outputs_Internal!L$50/12</f>
@@ -4768,15 +4804,15 @@
       </c>
       <c r="M19" s="67">
         <f>$F19*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N19" s="67">
         <f>$F19*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O19" s="67">
         <f>$F19*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P19" s="67">
         <f>$F19*Outputs_Internal!L$50/12</f>
@@ -4834,15 +4870,15 @@
       </c>
       <c r="M20" s="67">
         <f>$F20*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N20" s="67">
         <f>$F20*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O20" s="67">
         <f>$F20*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P20" s="67">
         <f>$F20*Outputs_Internal!L$50/12</f>
@@ -4850,15 +4886,15 @@
       </c>
       <c r="R20" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S20" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T20" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U20" s="67">
         <f t="shared" si="5"/>
@@ -4900,15 +4936,15 @@
       </c>
       <c r="M21" s="67">
         <f>$F21*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N21" s="67">
         <f>$F21*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O21" s="67">
         <f>$F21*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P21" s="67">
         <f>$F21*Outputs_Internal!L$50/12</f>
@@ -4966,15 +5002,15 @@
       </c>
       <c r="M22" s="67">
         <f>$F22*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N22" s="67">
         <f>$F22*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O22" s="67">
         <f>$F22*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P22" s="67">
         <f>$F22*Outputs_Internal!L$50/12</f>
@@ -5032,15 +5068,15 @@
       </c>
       <c r="M23" s="67">
         <f>$F23*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N23" s="67">
         <f>$F23*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O23" s="67">
         <f>$F23*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P23" s="67">
         <f>$F23*Outputs_Internal!L$50/12</f>
@@ -5048,15 +5084,15 @@
       </c>
       <c r="R23" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S23" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T23" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U23" s="67">
         <f t="shared" si="5"/>
@@ -5098,15 +5134,15 @@
       </c>
       <c r="M24" s="67">
         <f>$F24*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N24" s="67">
         <f>$F24*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O24" s="67">
         <f>$F24*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P24" s="67">
         <f>$F24*Outputs_Internal!L$50/12</f>
@@ -5164,15 +5200,15 @@
       </c>
       <c r="M25" s="67">
         <f>$F25*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N25" s="67">
         <f>$F25*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O25" s="67">
         <f>$F25*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P25" s="67">
         <f>$F25*Outputs_Internal!L$50/12</f>
@@ -5230,15 +5266,15 @@
       </c>
       <c r="M26" s="67">
         <f>$F26*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N26" s="67">
         <f>$F26*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O26" s="67">
         <f>$F26*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P26" s="67">
         <f>$F26*Outputs_Internal!L$50/12</f>
@@ -5246,15 +5282,15 @@
       </c>
       <c r="R26" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S26" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T26" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U26" s="67">
         <f t="shared" si="5"/>
@@ -5296,15 +5332,15 @@
       </c>
       <c r="M27" s="67">
         <f>$F27*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N27" s="67">
         <f>$F27*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O27" s="67">
         <f>$F27*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P27" s="67">
         <f>$F27*Outputs_Internal!L$50/12</f>
@@ -5362,15 +5398,15 @@
       </c>
       <c r="M28" s="67">
         <f>$F28*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N28" s="67">
         <f>$F28*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O28" s="67">
         <f>$F28*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P28" s="67">
         <f>$F28*Outputs_Internal!L$50/12</f>
@@ -5428,15 +5464,15 @@
       </c>
       <c r="M29" s="67">
         <f>$F29*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N29" s="67">
         <f>$F29*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O29" s="67">
         <f>$F29*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P29" s="67">
         <f>$F29*Outputs_Internal!L$50/12</f>
@@ -5444,15 +5480,15 @@
       </c>
       <c r="R29" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S29" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T29" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U29" s="67">
         <f t="shared" si="5"/>
@@ -5494,15 +5530,15 @@
       </c>
       <c r="M30" s="67">
         <f>$F30*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N30" s="67">
         <f>$F30*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O30" s="67">
         <f>$F30*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P30" s="67">
         <f>$F30*Outputs_Internal!L$50/12</f>
@@ -5560,15 +5596,15 @@
       </c>
       <c r="M31" s="67">
         <f>$F31*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N31" s="67">
         <f>$F31*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O31" s="67">
         <f>$F31*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P31" s="67">
         <f>$F31*Outputs_Internal!L$50/12</f>
@@ -5626,15 +5662,15 @@
       </c>
       <c r="M32" s="67">
         <f>$F32*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N32" s="67">
         <f>$F32*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O32" s="67">
         <f>$F32*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P32" s="67">
         <f>$F32*Outputs_Internal!L$50/12</f>
@@ -5642,15 +5678,15 @@
       </c>
       <c r="R32" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S32" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T32" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U32" s="67">
         <f t="shared" si="5"/>
@@ -5692,15 +5728,15 @@
       </c>
       <c r="M33" s="67">
         <f>$F33*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N33" s="67">
         <f>$F33*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O33" s="67">
         <f>$F33*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P33" s="67">
         <f>$F33*Outputs_Internal!L$50/12</f>
@@ -5758,15 +5794,15 @@
       </c>
       <c r="M34" s="67">
         <f>$F34*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N34" s="67">
         <f>$F34*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O34" s="67">
         <f>$F34*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P34" s="67">
         <f>$F34*Outputs_Internal!L$50/12</f>
@@ -5824,15 +5860,15 @@
       </c>
       <c r="M35" s="67">
         <f>$F35*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N35" s="67">
         <f>$F35*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O35" s="67">
         <f>$F35*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P35" s="67">
         <f>$F35*Outputs_Internal!L$50/12</f>
@@ -5840,15 +5876,15 @@
       </c>
       <c r="R35" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S35" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T35" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U35" s="67">
         <f t="shared" si="5"/>
@@ -5890,15 +5926,15 @@
       </c>
       <c r="M36" s="67">
         <f>$F36*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N36" s="67">
         <f>$F36*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O36" s="67">
         <f>$F36*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P36" s="67">
         <f>$F36*Outputs_Internal!L$50/12</f>
@@ -5956,15 +5992,15 @@
       </c>
       <c r="M37" s="67">
         <f>$F37*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N37" s="67">
         <f>$F37*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O37" s="67">
         <f>$F37*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P37" s="67">
         <f>$F37*Outputs_Internal!L$50/12</f>
@@ -6022,15 +6058,15 @@
       </c>
       <c r="M38" s="67">
         <f>$F38*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N38" s="67">
         <f>$F38*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O38" s="67">
         <f>$F38*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P38" s="67">
         <f>$F38*Outputs_Internal!L$50/12</f>
@@ -6038,15 +6074,15 @@
       </c>
       <c r="R38" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S38" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T38" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U38" s="67">
         <f t="shared" si="5"/>
@@ -6088,15 +6124,15 @@
       </c>
       <c r="M39" s="67">
         <f>$F39*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N39" s="67">
         <f>$F39*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O39" s="67">
         <f>$F39*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P39" s="67">
         <f>$F39*Outputs_Internal!L$50/12</f>
@@ -6154,15 +6190,15 @@
       </c>
       <c r="M40" s="67">
         <f>$F40*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N40" s="67">
         <f>$F40*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O40" s="67">
         <f>$F40*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P40" s="67">
         <f>$F40*Outputs_Internal!L$50/12</f>
@@ -6220,15 +6256,15 @@
       </c>
       <c r="M41" s="67">
         <f>$F41*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N41" s="67">
         <f>$F41*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O41" s="67">
         <f>$F41*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P41" s="67">
         <f>$F41*Outputs_Internal!L$50/12</f>
@@ -6236,15 +6272,15 @@
       </c>
       <c r="R41" s="67">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S41" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T41" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U41" s="67">
         <f t="shared" si="5"/>
@@ -6286,15 +6322,15 @@
       </c>
       <c r="M42" s="67">
         <f>$F42*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N42" s="67">
         <f>$F42*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O42" s="67">
         <f>$F42*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P42" s="67">
         <f>$F42*Outputs_Internal!L$50/12</f>
@@ -6352,15 +6388,15 @@
       </c>
       <c r="M43" s="67">
         <f>$F43*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N43" s="67">
         <f>$F43*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O43" s="67">
         <f>$F43*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P43" s="67">
         <f>$F43*Outputs_Internal!L$50/12</f>
@@ -6418,15 +6454,15 @@
       </c>
       <c r="M44" s="67">
         <f>$F44*Outputs_Internal!$D$50/12</f>
-        <v>0</v>
+        <v>3925</v>
       </c>
       <c r="N44" s="67">
         <f>$F44*Outputs_Internal!J$50/12</f>
-        <v>0</v>
+        <v>1685</v>
       </c>
       <c r="O44" s="67">
         <f>$F44*Outputs_Internal!K$50/12</f>
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="P44" s="67">
         <f>$F44*Outputs_Internal!L$50/12</f>
@@ -6434,15 +6470,15 @@
       </c>
       <c r="R44" s="67">
         <f>IF(MOD(MONTH($B44),3)=0,SUM(H42:H44,M42:M44),0)</f>
-        <v>0</v>
+        <v>11775</v>
       </c>
       <c r="S44" s="67">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5055</v>
       </c>
       <c r="T44" s="67">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6720</v>
       </c>
       <c r="U44" s="67">
         <f t="shared" si="5"/>
@@ -9822,7 +9858,7 @@
       </c>
       <c r="D4" s="1">
         <f>IF(AND(Inputs!D5="Y",Inputs!D4="Y"), 0, IF(Inputs!D4="Y", SUM(Prices!$C$3, IF(Inputs!D$6 ="Y", Prices!$C$4, 0)), IF(Inputs!D4="N", Prices!$D$3, 0)))</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="1">
         <f>IF(AND(Inputs!E5="Y",Inputs!E4="Y"), 0, IF(Inputs!E4="Y", SUM(Prices!$C$3, IF(Inputs!E$6 ="Y", Prices!$C$4, 0)), IF(Inputs!E4="N", Prices!$D$3, 0)))</f>
@@ -9891,7 +9927,7 @@
       </c>
       <c r="D9" s="16">
         <f>IF(Inputs!D4="Y", Prices!$C$6, IF(Inputs!D4="N", Prices!$D$6, 0))</f>
-        <v>0</v>
+        <v>18000</v>
       </c>
       <c r="E9" s="16">
         <f>IF(Inputs!E4="Y", Prices!$C$6, IF(Inputs!E4="N", Prices!$D$6, 0))</f>
@@ -9916,7 +9952,7 @@
       </c>
       <c r="D10" s="16">
         <f>IF(Inputs!D8="Y", Prices!$C$7, 0)</f>
-        <v>0</v>
+        <v>8100</v>
       </c>
       <c r="E10" s="16">
         <f>IF(Inputs!E8="Y", Prices!$C$7, 0)</f>
@@ -9941,7 +9977,7 @@
       </c>
       <c r="D11" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D9="Y",Inputs!D$19="Y"), Prices!$C10, 0)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="E11" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E9="Y",Inputs!E$19="Y"), Prices!$C10, 0)</f>
@@ -9966,7 +10002,7 @@
       </c>
       <c r="D12" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D10="Y",Inputs!D$19="Y"), Prices!$C11, 0)</f>
-        <v>0</v>
+        <v>4800</v>
       </c>
       <c r="E12" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E10="Y",Inputs!E$19="Y"), Prices!$C11, 0)</f>
@@ -9991,7 +10027,7 @@
       </c>
       <c r="D13" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$19="Y"), Prices!$C12, 0)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="E13" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E11="Y",Inputs!E$19="Y"), Prices!$C12, 0)</f>
@@ -10016,7 +10052,7 @@
       </c>
       <c r="D14" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D12="Y",Inputs!D$19="Y"), Prices!$C13, 0)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="E14" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!E12="Y",Inputs!E$19="Y"), Prices!$C13, 0)</f>
@@ -10448,7 +10484,7 @@
       </c>
       <c r="D35" s="16">
         <f>IF(Inputs!D4="Y", Prices!$C$6, IF(Inputs!D4="N", Prices!$D$6, 0))</f>
-        <v>0</v>
+        <v>18000</v>
       </c>
       <c r="E35" s="16">
         <f>IF(Inputs!E4="Y", Prices!$C$6, IF(Inputs!E4="N", Prices!$D$6, 0))</f>
@@ -10473,7 +10509,7 @@
       </c>
       <c r="D36" s="16">
         <f>IF(Inputs!D8="Y", Prices!$C$7, 0)</f>
-        <v>0</v>
+        <v>8100</v>
       </c>
       <c r="E36" s="16">
         <f>IF(Inputs!E8="Y", Prices!$C$7, 0)</f>
@@ -10498,7 +10534,7 @@
       </c>
       <c r="D37" s="18">
         <f>IF(AND(Inputs!D9="Y",Inputs!D$19="N"),Prices!$C10,0)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="E37" s="18">
         <f>IF(AND(Inputs!E9="Y",Inputs!E$19="N"),Prices!$C10,0)</f>
@@ -10523,7 +10559,7 @@
       </c>
       <c r="D38" s="18">
         <f>IF(AND(Inputs!D10="Y",Inputs!D$19="N"),Prices!$C11,0)</f>
-        <v>0</v>
+        <v>4800</v>
       </c>
       <c r="E38" s="18">
         <f>IF(AND(Inputs!E10="Y",Inputs!E$19="N"),Prices!$C11,0)</f>
@@ -10548,7 +10584,7 @@
       </c>
       <c r="D39" s="18">
         <f>IF(AND(Inputs!D11="Y",Inputs!D$19="N"),Prices!$C12,0)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="E39" s="18">
         <f>IF(AND(Inputs!E11="Y",Inputs!E$19="N"),Prices!$C12,0)</f>
@@ -10573,7 +10609,7 @@
       </c>
       <c r="D40" s="18">
         <f>IF(AND(Inputs!D12="Y",Inputs!D$19="N"),Prices!$C13,0)</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="E40" s="18">
         <f>IF(AND(Inputs!E12="Y",Inputs!E$19="N"),Prices!$C13,0)</f>
@@ -10998,7 +11034,7 @@
       </c>
       <c r="D61" s="18">
         <f>IF(Inputs!D$19 = "Y", 0, IF(Inputs!D18="Y", Prices!$C20, 0))</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="E61" s="18">
         <f>IF(Inputs!E$19 = "Y", 0, IF(Inputs!E18="Y", Prices!$C20, 0))</f>
@@ -11063,7 +11099,7 @@
       </c>
       <c r="K62" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L62" s="21">
         <f t="shared" ref="L62:L64" si="4">IF(COUNTIF(E$61:E$64,"")&gt;2,"",IFERROR(RANK(E62,E$61:E$64),4))</f>
@@ -11108,7 +11144,7 @@
       </c>
       <c r="K63" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L63" s="21">
         <f t="shared" si="4"/>
@@ -11153,7 +11189,7 @@
       </c>
       <c r="K64" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L64" s="21">
         <f t="shared" si="4"/>
@@ -11198,7 +11234,7 @@
       </c>
       <c r="K67" s="21">
         <f t="shared" ref="K67" si="5">IF(COUNTIF(D$61:D$64,"")&gt;2,"",IFERROR(RANK(D67,D$61:D$64),4))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L67" s="21">
         <f>IF(COUNTIF(E$61:E$64,"")&gt;2,"",IFERROR(RANK(E67,E$61:E$64),4))</f>
@@ -11310,7 +11346,7 @@
       </c>
       <c r="D73" s="18">
         <f>D61</f>
-        <v>0</v>
+        <v>10200</v>
       </c>
       <c r="E73" s="18">
         <f t="shared" ref="E73:H73" si="9">E61</f>
@@ -11430,7 +11466,7 @@
       </c>
       <c r="K79" s="21">
         <f t="shared" ref="K79" si="13">IF(COUNTIF(D$61:D$64,"")&gt;2,"",IFERROR(RANK(D79,D$61:D$64),4))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L79" s="21">
         <f>IF(COUNTIF(E$61:E$64,"")&gt;2,"",IFERROR(RANK(E79,E$61:E$64),4))</f>
@@ -11585,7 +11621,7 @@
       </c>
       <c r="D88" s="7">
         <f>SUM(D35:D45, D48:D58, D61:D64, D67:D70, D85:D86)</f>
-        <v>0</v>
+        <v>47100</v>
       </c>
       <c r="E88" s="7">
         <f t="shared" ref="E88:H88" si="20">SUM(E35:E45, E48:E58, E61:E64, E67:E70, E85:E86)</f>
@@ -11638,7 +11674,7 @@
       </c>
       <c r="D92" s="7">
         <f>SUM(D88, D90)</f>
-        <v>0</v>
+        <v>47100</v>
       </c>
       <c r="E92" s="7">
         <f>SUM(E88, E90)</f>
@@ -11668,19 +11704,19 @@
       </c>
       <c r="E95" s="21">
         <f t="shared" ref="E95:H95" si="22">IFERROR(_xlfn.RANK.EQ(E88,$D$88:$H$88),5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F95" s="21">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G95" s="21">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H95" s="21">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -11709,19 +11745,19 @@
       </c>
       <c r="E97" s="21">
         <f t="shared" ref="E97:H97" si="23">SUM(E95:E96)</f>
-        <v>1.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F97" s="21">
         <f t="shared" si="23"/>
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G97" s="21">
         <f t="shared" si="23"/>
-        <v>1.4</v>
+        <v>2.4</v>
       </c>
       <c r="H97" s="21">
         <f t="shared" si="23"/>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="98" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Convert CCHGs to Medical Conditions.
Do this because we're not going to offer CCHGs.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scratch\todays_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="2"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Waste Calculator</t>
-  </si>
-  <si>
-    <t>CCHGs</t>
   </si>
   <si>
     <t>PRM Oppourtunity Prospective Scores</t>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t>Royalties</t>
+  </si>
+  <si>
+    <t>Medical Conditions</t>
   </si>
 </sst>
 </file>
@@ -1018,59 +1018,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
     <col min="3" max="3" width="18" style="70" customWidth="1"/>
-    <col min="4" max="8" width="18.7109375" customWidth="1"/>
+    <col min="4" max="8" width="18.7265625" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B1" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" s="76">
         <v>43101</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="77">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="73"/>
       <c r="C3" s="78"/>
       <c r="D3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="74" t="s">
         <v>6</v>
       </c>
@@ -1085,34 +1085,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="74" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="56"/>
       <c r="F5" s="56"/>
       <c r="G5" s="56"/>
       <c r="H5" s="57"/>
       <c r="L5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="74" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="56"/>
       <c r="F6" s="56"/>
       <c r="G6" s="56"/>
       <c r="H6" s="57"/>
     </row>
-    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="74" t="s">
         <v>5</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="G7" s="56"/>
       <c r="H7" s="57"/>
     </row>
-    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="74" t="s">
         <v>9</v>
       </c>
@@ -1136,7 +1136,7 @@
       <c r="G8" s="56"/>
       <c r="H8" s="57"/>
     </row>
-    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="74" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="G9" s="56"/>
       <c r="H9" s="57"/>
     </row>
-    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="74" t="s">
         <v>11</v>
       </c>
@@ -1160,9 +1160,9 @@
       <c r="G10" s="56"/>
       <c r="H10" s="57"/>
     </row>
-    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="74" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="56" t="s">
         <v>4</v>
@@ -1172,7 +1172,7 @@
       <c r="G11" s="56"/>
       <c r="H11" s="57"/>
     </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="74" t="s">
         <v>12</v>
       </c>
@@ -1184,69 +1184,69 @@
       <c r="G12" s="56"/>
       <c r="H12" s="57"/>
     </row>
-    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="74" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="56"/>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
       <c r="H13" s="57"/>
     </row>
-    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="74" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
       <c r="H14" s="57"/>
     </row>
-    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="56"/>
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
       <c r="H15" s="57"/>
     </row>
-    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="56"/>
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
       <c r="H16" s="57"/>
     </row>
-    <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="56"/>
       <c r="F17" s="56"/>
       <c r="G17" s="56"/>
       <c r="H17" s="57"/>
     </row>
-    <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="56" t="s">
         <v>4</v>
@@ -1256,37 +1256,37 @@
       <c r="G18" s="56"/>
       <c r="H18" s="57"/>
     </row>
-    <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" s="56"/>
       <c r="F19" s="56"/>
       <c r="G19" s="56"/>
       <c r="H19" s="57"/>
     </row>
-    <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="74" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="56"/>
       <c r="F20" s="56"/>
       <c r="G20" s="56"/>
       <c r="H20" s="57"/>
     </row>
-    <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="71"/>
       <c r="D21" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="58"/>
       <c r="F21" s="58"/>
@@ -1318,45 +1318,45 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.26953125" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1402,12 +1402,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C8" s="15" t="s">
         <v>3</v>
       </c>
@@ -1479,9 +1479,9 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C9" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="18">
         <f>SUM(Calcs!D37, Calcs!D50)</f>
@@ -1515,7 +1515,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C10" s="17" t="s">
         <v>11</v>
       </c>
@@ -1551,9 +1551,9 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="18">
         <f>SUM(Calcs!D39, Calcs!D52)</f>
@@ -1586,7 +1586,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
         <v>12</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
         <v>13</v>
       </c>
@@ -1656,9 +1656,9 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C14" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D14" s="18">
         <f>SUM(Calcs!D42, Calcs!D55)</f>
@@ -1691,9 +1691,9 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C15" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="20">
         <f>SUM(Calcs!D43, Calcs!D56)</f>
@@ -1726,9 +1726,9 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C16" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="20">
         <f>SUM(Calcs!D44, Calcs!D57)</f>
@@ -1761,9 +1761,9 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C17" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(Calcs!D45, Calcs!D58)</f>
@@ -1796,14 +1796,14 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1">
         <f>SUM(Calcs!D61, Calcs!D67)</f>
@@ -1836,9 +1836,9 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1">
         <f>SUM(Calcs!D62, Calcs!D68)</f>
@@ -1871,9 +1871,9 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1">
         <f>SUM(Calcs!D63, Calcs!D69)</f>
@@ -1906,9 +1906,9 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(Calcs!D64, Calcs!D70)</f>
@@ -1941,14 +1941,14 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>61</v>
       </c>
       <c r="D26" s="1">
         <f>SUM(Calcs!D85:D86)</f>
@@ -1981,9 +1981,9 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="1">
         <f>Calcs!D90</f>
@@ -2016,9 +2016,9 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D29" s="7">
         <f>SUM(D7:D17, D20:D23, D26:D27)</f>
@@ -2048,7 +2048,7 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2062,9 +2062,9 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B31" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -2082,15 +2082,15 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C32" s="68">
         <f>INDEX(Outputs_Timeline!$D$3:$D$94,MATCH(Inputs!$C$1,Outputs_Timeline!$B$3:$B$94,0),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="7">
         <f>(D29/12*Inputs!$C$2+D4)*$C$32</f>
@@ -2120,7 +2120,7 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2135,18 +2135,18 @@
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C38" s="7">
         <f>SUM(Outputs_Timeline!R:R)</f>
         <v>146300</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C39" s="53">
         <f>SUM(D34:H34)</f>
         <v>146300</v>
@@ -2154,17 +2154,17 @@
       <c r="D39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D41" s="2"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -2181,67 +2181,67 @@
   </sheetPr>
   <dimension ref="B1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:L55"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+    <col min="9" max="9" width="3.81640625" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F1" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" s="51"/>
       <c r="H1" s="51"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D2" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="H2" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="L2" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="1">
         <f>SUMIF(Inputs!$D$4:$H$4, "Y", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -2271,9 +2271,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1">
         <f>SUMIF(Inputs!$D$4:$H$4, "N", Outputs_External!D4:'Outputs_External'!H4)</f>
@@ -2303,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="26"/>
@@ -2311,9 +2311,9 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -2322,7 +2322,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C8" s="15" t="s">
         <v>2</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C9" s="15" t="s">
         <v>3</v>
       </c>
@@ -2386,9 +2386,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C10" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="18">
         <f>SUM(Calcs!D11:H11)</f>
@@ -2418,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
         <v>11</v>
       </c>
@@ -2450,9 +2450,9 @@
         <v>479.99999999999989</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="18">
         <f>SUM(Calcs!D13:H13)</f>
@@ -2481,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
         <v>12</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C14" s="17" t="s">
         <v>13</v>
       </c>
@@ -2543,23 +2543,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C15" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D15" s="18">
         <f>SUM(Calcs!D16:H16)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="G15" s="33">
-        <v>0.1</v>
+      <c r="F15" s="80">
+        <v>0.6</v>
+      </c>
+      <c r="G15" s="80">
+        <v>0.4</v>
       </c>
       <c r="H15" s="37">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J15" s="18">
         <f t="shared" si="3"/>
@@ -2574,9 +2574,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C16" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="20">
         <f>SUM(Calcs!D17:H17)</f>
@@ -2605,9 +2605,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C17" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(Calcs!D18:H18)</f>
@@ -2636,9 +2636,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C18" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="20">
         <f>SUM(Calcs!D19:H19)</f>
@@ -2667,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -2675,9 +2675,9 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="G20" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" s="10">
         <v>0.1</v>
@@ -2686,7 +2686,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2694,9 +2694,9 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -2705,7 +2705,7 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C23" s="15" t="s">
         <v>2</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C24" s="28" t="s">
         <v>3</v>
       </c>
@@ -2773,9 +2773,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C25" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="18">
         <f>SUM(Calcs!D24:H24)</f>
@@ -2807,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C26" s="17" t="s">
         <v>11</v>
       </c>
@@ -2841,9 +2841,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C27" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="18">
         <f>SUM(Calcs!D26:H26)</f>
@@ -2874,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C28" s="17" t="s">
         <v>12</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C29" s="17" t="s">
         <v>13</v>
       </c>
@@ -2940,9 +2940,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C30" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D30" s="18">
         <f>SUM(Calcs!D29:H29)</f>
@@ -2950,15 +2950,15 @@
       </c>
       <c r="F30" s="37">
         <f t="shared" si="8"/>
-        <v>8.8888888888888906E-2</v>
+        <v>0.5</v>
       </c>
       <c r="G30" s="37">
         <f t="shared" si="5"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H30" s="37">
         <f t="shared" si="9"/>
-        <v>0.71111111111111125</v>
+        <v>0</v>
       </c>
       <c r="J30" s="18">
         <f t="shared" si="10"/>
@@ -2973,9 +2973,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C31" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" s="20">
         <f>SUM(Calcs!D30:H30)</f>
@@ -3006,9 +3006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C32" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="20">
         <f>SUM(Calcs!D31:H31)</f>
@@ -3039,9 +3039,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C33" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" s="29">
         <f>SUM(Calcs!D32:H32)</f>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
@@ -3080,9 +3080,9 @@
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -3091,9 +3091,9 @@
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C36" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="18">
         <f>SUM(Calcs!D73:H73)</f>
@@ -3122,9 +3122,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C37" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" s="18">
         <f>SUM(Calcs!D74:H74)</f>
@@ -3153,9 +3153,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C38" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38" s="20">
         <f>SUM(Calcs!D75:H75)</f>
@@ -3184,9 +3184,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C39" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" s="20">
         <f>SUM(Calcs!D76:H76)</f>
@@ -3215,14 +3215,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B41" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -3231,9 +3231,9 @@
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C42" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" s="29">
         <f>SUM(Calcs!D79:H79)</f>
@@ -3264,9 +3264,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C43" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43" s="18">
         <f>SUM(Calcs!D80:H80)</f>
@@ -3297,9 +3297,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C44" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="20">
         <f>SUM(Calcs!D81:H81)</f>
@@ -3330,9 +3330,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C45" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D45" s="20">
         <f>SUM(Calcs!D82:H82)</f>
@@ -3363,22 +3363,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B47" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="1">
         <f>SUM(Outputs_External!D26:'Outputs_External'!H26)</f>
@@ -3409,9 +3409,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1">
         <f>SUM(Outputs_External!D27:'Outputs_External'!H27)</f>
@@ -3442,14 +3442,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B51" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" s="1">
         <f>SUM(Outputs_External!D29:'Outputs_External'!H29)</f>
@@ -3468,9 +3468,9 @@
         <v>479.99999999999989</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C52" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D52" s="23">
         <f>SUM(J51:L51)</f>
@@ -3480,14 +3480,14 @@
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B54" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" s="1">
         <f>SUM(Outputs_Timeline!R:R)</f>
@@ -3506,7 +3506,7 @@
         <v>1439.9999999999998</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D55" s="1"/>
       <c r="J55" s="54">
         <f>IFERROR(J54/$D$54, 0)</f>
@@ -3521,14 +3521,14 @@
         <v>9.8427887901572104E-3</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B58" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="21"/>
@@ -3541,10 +3541,10 @@
       <c r="K58" s="22"/>
       <c r="L58" s="22"/>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B59" s="27"/>
       <c r="C59" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" s="23">
         <f>SUM(Calcs!D61:H61)+SUM(Calcs!D67:H67)</f>
@@ -3577,10 +3577,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B60" s="27"/>
       <c r="C60" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D60" s="23">
         <f>SUM(Calcs!D62:H62)+SUM(Calcs!D68:H68)</f>
@@ -3613,10 +3613,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B61" s="27"/>
       <c r="C61" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D61" s="23">
         <f>SUM(Calcs!D63:H63)+SUM(Calcs!D69:H69)</f>
@@ -3649,10 +3649,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B62" s="27"/>
       <c r="C62" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D62" s="23">
         <f>SUM(Calcs!D64:H64)+SUM(Calcs!D70:H70)</f>
@@ -3699,102 +3699,102 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="64" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="64" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="64" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="64" customWidth="1"/>
-    <col min="8" max="11" width="8.7109375" style="67"/>
-    <col min="12" max="12" width="5.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="67" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="8.7109375" style="67"/>
-    <col min="17" max="17" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.453125" style="64" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="64" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.54296875" style="64" customWidth="1"/>
+    <col min="8" max="11" width="8.7265625" style="67"/>
+    <col min="12" max="12" width="5.453125" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="67" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="8.7265625" style="67"/>
+    <col min="17" max="17" width="3.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.35">
       <c r="F1" s="69">
         <f>COUNTIF(F3:F94,"&gt;0")</f>
         <v>36</v>
       </c>
       <c r="H1" s="65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" s="65"/>
       <c r="J1" s="65"/>
       <c r="K1" s="65"/>
       <c r="M1" s="65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
       <c r="P1" s="65"/>
       <c r="R1" s="65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S1" s="65"/>
       <c r="T1" s="65"/>
       <c r="U1" s="65"/>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B2" s="63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="63"/>
       <c r="D2" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="63"/>
       <c r="H2" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="66" t="s">
+      <c r="J2" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="66" t="s">
-        <v>90</v>
-      </c>
       <c r="M2" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="N2" s="66" t="s">
+      <c r="O2" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" s="66" t="s">
-        <v>90</v>
-      </c>
       <c r="R2" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="66" t="s">
+      <c r="T2" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="T2" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="66" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" s="64">
         <v>42917</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="T3" s="67"/>
       <c r="U3" s="67"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B4" s="64">
         <f>EDATE(B3,1)</f>
         <v>42948</v>
@@ -3897,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" s="64">
         <f t="shared" ref="B5:B68" si="0">EDATE(B4,1)</f>
         <v>42979</v>
@@ -3963,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="64">
         <f t="shared" si="0"/>
         <v>43009</v>
@@ -4029,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B7" s="64">
         <f t="shared" si="0"/>
         <v>43040</v>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B8" s="64">
         <f t="shared" si="0"/>
         <v>43070</v>
@@ -4161,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B9" s="64">
         <f t="shared" si="0"/>
         <v>43101</v>
@@ -4227,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" s="64">
         <f t="shared" si="0"/>
         <v>43132</v>
@@ -4293,7 +4293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" s="64">
         <f t="shared" si="0"/>
         <v>43160</v>
@@ -4359,7 +4359,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B12" s="64">
         <f t="shared" si="0"/>
         <v>43191</v>
@@ -4425,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B13" s="64">
         <f t="shared" si="0"/>
         <v>43221</v>
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" s="64">
         <f t="shared" si="0"/>
         <v>43252</v>
@@ -4557,7 +4557,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" s="64">
         <f t="shared" si="0"/>
         <v>43282</v>
@@ -4623,7 +4623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B16" s="64">
         <f t="shared" si="0"/>
         <v>43313</v>
@@ -4689,7 +4689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B17" s="64">
         <f t="shared" si="0"/>
         <v>43344</v>
@@ -4755,7 +4755,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" s="64">
         <f t="shared" si="0"/>
         <v>43374</v>
@@ -4821,7 +4821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="64">
         <f t="shared" si="0"/>
         <v>43405</v>
@@ -4887,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B20" s="64">
         <f t="shared" si="0"/>
         <v>43435</v>
@@ -4953,7 +4953,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B21" s="64">
         <f t="shared" si="0"/>
         <v>43466</v>
@@ -5019,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B22" s="64">
         <f t="shared" si="0"/>
         <v>43497</v>
@@ -5085,7 +5085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B23" s="64">
         <f t="shared" si="0"/>
         <v>43525</v>
@@ -5151,7 +5151,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B24" s="64">
         <f t="shared" si="0"/>
         <v>43556</v>
@@ -5217,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B25" s="64">
         <f t="shared" si="0"/>
         <v>43586</v>
@@ -5283,7 +5283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B26" s="64">
         <f t="shared" si="0"/>
         <v>43617</v>
@@ -5349,7 +5349,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B27" s="64">
         <f t="shared" si="0"/>
         <v>43647</v>
@@ -5415,7 +5415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B28" s="64">
         <f t="shared" si="0"/>
         <v>43678</v>
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B29" s="64">
         <f t="shared" si="0"/>
         <v>43709</v>
@@ -5547,7 +5547,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B30" s="64">
         <f t="shared" si="0"/>
         <v>43739</v>
@@ -5613,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B31" s="64">
         <f t="shared" si="0"/>
         <v>43770</v>
@@ -5679,7 +5679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B32" s="64">
         <f t="shared" si="0"/>
         <v>43800</v>
@@ -5745,7 +5745,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B33" s="64">
         <f t="shared" si="0"/>
         <v>43831</v>
@@ -5811,7 +5811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B34" s="64">
         <f t="shared" si="0"/>
         <v>43862</v>
@@ -5877,7 +5877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B35" s="64">
         <f t="shared" si="0"/>
         <v>43891</v>
@@ -5943,7 +5943,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B36" s="64">
         <f t="shared" si="0"/>
         <v>43922</v>
@@ -6009,7 +6009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B37" s="64">
         <f t="shared" si="0"/>
         <v>43952</v>
@@ -6075,7 +6075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B38" s="64">
         <f t="shared" si="0"/>
         <v>43983</v>
@@ -6141,7 +6141,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B39" s="64">
         <f t="shared" si="0"/>
         <v>44013</v>
@@ -6207,7 +6207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B40" s="64">
         <f t="shared" si="0"/>
         <v>44044</v>
@@ -6273,7 +6273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B41" s="64">
         <f t="shared" si="0"/>
         <v>44075</v>
@@ -6339,7 +6339,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B42" s="64">
         <f t="shared" si="0"/>
         <v>44105</v>
@@ -6405,7 +6405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B43" s="64">
         <f t="shared" si="0"/>
         <v>44136</v>
@@ -6471,7 +6471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B44" s="64">
         <f t="shared" si="0"/>
         <v>44166</v>
@@ -6537,7 +6537,7 @@
         <v>119.99999999999997</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B45" s="64">
         <f t="shared" si="0"/>
         <v>44197</v>
@@ -6603,7 +6603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B46" s="64">
         <f t="shared" si="0"/>
         <v>44228</v>
@@ -6669,7 +6669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B47" s="64">
         <f t="shared" si="0"/>
         <v>44256</v>
@@ -6735,7 +6735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B48" s="64">
         <f t="shared" si="0"/>
         <v>44287</v>
@@ -6801,7 +6801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B49" s="64">
         <f t="shared" si="0"/>
         <v>44317</v>
@@ -6867,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B50" s="64">
         <f t="shared" si="0"/>
         <v>44348</v>
@@ -6933,7 +6933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B51" s="64">
         <f t="shared" si="0"/>
         <v>44378</v>
@@ -6999,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B52" s="64">
         <f t="shared" si="0"/>
         <v>44409</v>
@@ -7065,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B53" s="64">
         <f t="shared" si="0"/>
         <v>44440</v>
@@ -7131,7 +7131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B54" s="64">
         <f t="shared" si="0"/>
         <v>44470</v>
@@ -7197,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B55" s="64">
         <f t="shared" si="0"/>
         <v>44501</v>
@@ -7263,7 +7263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B56" s="64">
         <f t="shared" si="0"/>
         <v>44531</v>
@@ -7329,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B57" s="64">
         <f t="shared" si="0"/>
         <v>44562</v>
@@ -7395,7 +7395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B58" s="64">
         <f t="shared" si="0"/>
         <v>44593</v>
@@ -7461,7 +7461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B59" s="64">
         <f t="shared" si="0"/>
         <v>44621</v>
@@ -7527,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B60" s="64">
         <f t="shared" si="0"/>
         <v>44652</v>
@@ -7593,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B61" s="64">
         <f t="shared" si="0"/>
         <v>44682</v>
@@ -7659,7 +7659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B62" s="64">
         <f t="shared" si="0"/>
         <v>44713</v>
@@ -7725,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B63" s="64">
         <f t="shared" si="0"/>
         <v>44743</v>
@@ -7791,7 +7791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B64" s="64">
         <f t="shared" si="0"/>
         <v>44774</v>
@@ -7857,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B65" s="64">
         <f t="shared" si="0"/>
         <v>44805</v>
@@ -7923,7 +7923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B66" s="64">
         <f t="shared" si="0"/>
         <v>44835</v>
@@ -7989,7 +7989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B67" s="64">
         <f t="shared" si="0"/>
         <v>44866</v>
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B68" s="64">
         <f t="shared" si="0"/>
         <v>44896</v>
@@ -8121,7 +8121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B69" s="64">
         <f t="shared" ref="B69:B94" si="6">EDATE(B68,1)</f>
         <v>44927</v>
@@ -8187,7 +8187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B70" s="64">
         <f t="shared" si="6"/>
         <v>44958</v>
@@ -8253,7 +8253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B71" s="64">
         <f t="shared" si="6"/>
         <v>44986</v>
@@ -8319,7 +8319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B72" s="64">
         <f t="shared" si="6"/>
         <v>45017</v>
@@ -8385,7 +8385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B73" s="64">
         <f t="shared" si="6"/>
         <v>45047</v>
@@ -8451,7 +8451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B74" s="64">
         <f t="shared" si="6"/>
         <v>45078</v>
@@ -8517,7 +8517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B75" s="64">
         <f t="shared" si="6"/>
         <v>45108</v>
@@ -8583,7 +8583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B76" s="64">
         <f t="shared" si="6"/>
         <v>45139</v>
@@ -8649,7 +8649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B77" s="64">
         <f t="shared" si="6"/>
         <v>45170</v>
@@ -8715,7 +8715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B78" s="64">
         <f t="shared" si="6"/>
         <v>45200</v>
@@ -8781,7 +8781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B79" s="64">
         <f t="shared" si="6"/>
         <v>45231</v>
@@ -8847,7 +8847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B80" s="64">
         <f t="shared" si="6"/>
         <v>45261</v>
@@ -8913,7 +8913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B81" s="64">
         <f t="shared" si="6"/>
         <v>45292</v>
@@ -8979,7 +8979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B82" s="64">
         <f t="shared" si="6"/>
         <v>45323</v>
@@ -9045,7 +9045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B83" s="64">
         <f t="shared" si="6"/>
         <v>45352</v>
@@ -9111,7 +9111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B84" s="64">
         <f t="shared" si="6"/>
         <v>45383</v>
@@ -9177,7 +9177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B85" s="64">
         <f t="shared" si="6"/>
         <v>45413</v>
@@ -9243,7 +9243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B86" s="64">
         <f t="shared" si="6"/>
         <v>45444</v>
@@ -9309,7 +9309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B87" s="64">
         <f t="shared" si="6"/>
         <v>45474</v>
@@ -9375,7 +9375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B88" s="64">
         <f t="shared" si="6"/>
         <v>45505</v>
@@ -9441,7 +9441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B89" s="64">
         <f t="shared" si="6"/>
         <v>45536</v>
@@ -9507,7 +9507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B90" s="64">
         <f t="shared" si="6"/>
         <v>45566</v>
@@ -9573,7 +9573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B91" s="64">
         <f t="shared" si="6"/>
         <v>45597</v>
@@ -9639,7 +9639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B92" s="64">
         <f t="shared" si="6"/>
         <v>45627</v>
@@ -9705,7 +9705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B93" s="64">
         <f t="shared" si="6"/>
         <v>45658</v>
@@ -9771,7 +9771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B94" s="64">
         <f t="shared" si="6"/>
         <v>45689</v>
@@ -9855,56 +9855,56 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" customWidth="1"/>
-    <col min="4" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" customWidth="1"/>
+    <col min="4" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="15" width="18" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
       <c r="K2" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="O2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -9929,16 +9929,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5">
         <f>IF(Inputs!D4="N",MAX(Inputs!D7-25000,0),0)</f>
@@ -9961,19 +9961,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C10" s="15" t="s">
         <v>3</v>
       </c>
@@ -10023,9 +10023,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C11" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D9="Y",Inputs!D$19="Y"), Prices!$C10, 0)</f>
@@ -10048,7 +10048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C12" s="17" t="s">
         <v>11</v>
       </c>
@@ -10073,9 +10073,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C13" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D11="Y",Inputs!D$19="Y"), Prices!$C12, 0)</f>
@@ -10098,7 +10098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C14" s="17" t="s">
         <v>12</v>
       </c>
@@ -10123,7 +10123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C15" s="17" t="s">
         <v>13</v>
       </c>
@@ -10148,9 +10148,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C16" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D16" s="18">
         <f xml:space="preserve"> IF(OR(Inputs!D14="Y",Inputs!D$19="Y"), Prices!$C15, 0)</f>
@@ -10173,9 +10173,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C17" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D15="Y",Inputs!D$20="Y"), Prices!$C16, 0)</f>
@@ -10198,9 +10198,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C18" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D16="Y",Inputs!D$20="Y"), Prices!$C17, 0)</f>
@@ -10223,9 +10223,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C19" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="20">
         <f xml:space="preserve"> IF(OR(Inputs!D17="Y",Inputs!D$20="Y"), Prices!$C18, 0)</f>
@@ -10248,12 +10248,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C22" s="15" t="s">
         <v>2</v>
       </c>
@@ -10278,7 +10278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C23" s="28" t="s">
         <v>3</v>
       </c>
@@ -10298,9 +10298,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C24" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D9="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D10),0))</f>
@@ -10323,7 +10323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C25" s="17" t="s">
         <v>11</v>
       </c>
@@ -10348,9 +10348,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C26" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D11="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D12),0))</f>
@@ -10373,7 +10373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C27" s="17" t="s">
         <v>12</v>
       </c>
@@ -10398,7 +10398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C28" s="17" t="s">
         <v>13</v>
       </c>
@@ -10423,9 +10423,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C29" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D29" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D14="Y",Inputs!D$19="Y"),PRODUCT(D$6, Prices!$D15),0))</f>
@@ -10448,9 +10448,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C30" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$20="Y"),PRODUCT(D$6, Prices!$D16),0))</f>
@@ -10473,9 +10473,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C31" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$20="Y"),PRODUCT(D$6, Prices!$D17),0))</f>
@@ -10498,9 +10498,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C32" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="29">
         <v>0</v>
@@ -10518,19 +10518,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C35" s="15" t="s">
         <v>2</v>
       </c>
@@ -10555,7 +10555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C36" s="15" t="s">
         <v>3</v>
       </c>
@@ -10580,9 +10580,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C37" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="18">
         <f>IF(AND(Inputs!D9="Y",Inputs!D$19="N"),Prices!$C10,0)</f>
@@ -10605,7 +10605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C38" s="17" t="s">
         <v>11</v>
       </c>
@@ -10630,9 +10630,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C39" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" s="18">
         <f>IF(AND(Inputs!D11="Y",Inputs!D$19="N"),Prices!$C12,0)</f>
@@ -10655,7 +10655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C40" s="17" t="s">
         <v>12</v>
       </c>
@@ -10680,7 +10680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C41" s="17" t="s">
         <v>13</v>
       </c>
@@ -10705,9 +10705,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C42" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D42" s="18">
         <f>IF(AND(Inputs!D14="Y",Inputs!D$19="N"),Prices!$C15,0)</f>
@@ -10730,9 +10730,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C43" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="20">
         <f>IF(AND(Inputs!D15="Y",Inputs!D$20="N"),Prices!$C16,0)</f>
@@ -10755,9 +10755,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C44" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="20">
         <f>IF(AND(Inputs!D16="Y",Inputs!D$20="N"),Prices!$C17,0)</f>
@@ -10780,9 +10780,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C45" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="20">
         <f>IF(AND(Inputs!D17="Y",Inputs!D$20="N"),Prices!$C18,0)</f>
@@ -10805,12 +10805,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C48" s="15" t="s">
         <v>2</v>
       </c>
@@ -10835,7 +10835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C49" s="28" t="s">
         <v>3</v>
       </c>
@@ -10855,9 +10855,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C50" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D50" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D9="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D10),0))</f>
@@ -10880,7 +10880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C51" s="17" t="s">
         <v>11</v>
       </c>
@@ -10905,9 +10905,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C52" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D52" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D11="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D12),0))</f>
@@ -10930,7 +10930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C53" s="17" t="s">
         <v>12</v>
       </c>
@@ -10955,7 +10955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C54" s="17" t="s">
         <v>13</v>
       </c>
@@ -10980,9 +10980,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C55" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="D55" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D14="Y",Inputs!D$19="N"),PRODUCT(D$6, Prices!$D15),0))</f>
@@ -11005,9 +11005,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C56" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D56" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$20="N"),PRODUCT(D$6, Prices!$D16),0))</f>
@@ -11030,9 +11030,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C57" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" s="20">
         <f>IF(OR(Inputs!D$4="Y", D$6 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$20="N"),PRODUCT(D$6, Prices!$D17),0))</f>
@@ -11055,9 +11055,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C58" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D58" s="29">
         <v>0</v>
@@ -11075,14 +11075,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B60" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C61" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" s="18">
         <f>IF(Inputs!D$19 = "Y", 0, IF(Inputs!D18="Y", Prices!$C20, 0))</f>
@@ -11125,9 +11125,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C62" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" s="18">
         <f>IF(Inputs!D19="Y", Prices!$C21, 0)</f>
@@ -11170,9 +11170,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C63" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63" s="20">
         <f>IF(Inputs!D20="Y", Prices!$C22, 0)</f>
@@ -11215,9 +11215,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C64" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D64" s="20">
         <f>IF(Inputs!D21="Y", Prices!$C23, 0)</f>
@@ -11260,14 +11260,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B66" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C67" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" s="29">
         <v>0</v>
@@ -11305,9 +11305,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C68" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D68" s="18">
         <f>IF(Inputs!D$4="Y", 0, IF(D$6 = "", 0, IF(Inputs!D19 = "Y", D$6*Prices!$D21, 0)))</f>
@@ -11330,9 +11330,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C69" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D69" s="20">
         <f>IF(Inputs!D$4="Y", 0, IF(D$6 = "", 0, IF(Inputs!D20 = "Y", D$6*Prices!$D22, 0)))</f>
@@ -11355,9 +11355,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C70" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D70" s="20">
         <f>IF(Inputs!D$4="Y", 0, IF(D$6 = "", 0, IF(Inputs!D21 = "Y", D$6*Prices!$D23, 0)))</f>
@@ -11380,21 +11380,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.35">
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B72" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C73" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D73" s="18">
         <f>D61</f>
@@ -11417,9 +11417,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C74" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D74" s="18">
         <f>IF(D62=0,0,D62-SUM(D11:D16))</f>
@@ -11442,9 +11442,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C75" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D75" s="20">
         <f>IF(D63=0,0,D63-SUM(D17:D19))</f>
@@ -11467,9 +11467,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C76" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D76" s="20">
         <f t="shared" ref="D76:H76" si="12">D64</f>
@@ -11492,14 +11492,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B78" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C79" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D79" s="29">
         <v>0</v>
@@ -11537,9 +11537,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C80" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D80" s="18">
         <f>IF(D68=0,0,D68-SUM(D24:D29))</f>
@@ -11562,9 +11562,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C81" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D81" s="20">
         <f>IF(D69=0,0,D69-SUM(D30:D31))</f>
@@ -11587,9 +11587,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C82" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D82" s="20">
         <f t="shared" ref="D82:H82" si="19">D70</f>
@@ -11612,14 +11612,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B84" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C85" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D85" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$61:D$64, MATCH(2, K$61:K$64, 0)), INDEX(D$66:D$70, MATCH(2, K$61:K$64, 0)))*Prices!$I$5*-1, 0)</f>
@@ -11642,9 +11642,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C86" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D86" s="1">
         <f>_xlfn.IFNA(SUM(INDEX(D$61:D$64, MATCH(3, K$61:K$64, 0)), INDEX(D$66:D$70, MATCH(3, K$61:K$64, 0)))*Prices!$I$5*-1, 0)</f>
@@ -11667,9 +11667,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B88" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D88" s="7">
         <f>SUM(D35:D45, D48:D58, D61:D64, D67:D70, D85:D86)</f>
@@ -11692,12 +11692,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B90" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D90" s="1">
         <f>IF(D98=1, 0, IF(D98=2, $E$101, IF(D98=3, $E$102, IF(D98=4, $E$103, IF(D98=5, $E$104, "")))))</f>
@@ -11720,9 +11720,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B92" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D92" s="7">
         <f>SUM(D88, D90)</f>
@@ -11745,10 +11745,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B95" s="27"/>
       <c r="C95" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D95" s="21">
         <f>IFERROR(_xlfn.RANK.EQ(D88,$D$88:$H$88),5)</f>
@@ -11771,7 +11771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B96" s="27"/>
       <c r="D96" s="21">
         <v>0.1</v>
@@ -11789,7 +11789,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B97" s="27"/>
       <c r="D97" s="21">
         <f>SUM(D95:D96)</f>
@@ -11812,7 +11812,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="98" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B98" s="27"/>
       <c r="D98" s="21">
         <f>_xlfn.RANK.EQ(D97, $D$97:$H$97, 5)</f>
@@ -11835,56 +11835,56 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B99" s="27"/>
     </row>
-    <row r="100" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B100" s="27"/>
       <c r="C100" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B101" s="27"/>
       <c r="D101" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E101" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(2, $D$98:$H$98, 0))*Prices!$I$10*-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B102" s="27"/>
       <c r="D102" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E102" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(3, $D$98:$H$98, 0))*Prices!$I$11*-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B103" s="27"/>
       <c r="D103" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E103" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(4, $D$98:$H$98, 0))*Prices!$I$11*-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B104" s="27"/>
       <c r="D104" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E104" s="23">
         <f>INDEX($D$88:$H$88, 1, MATCH(5, $D$98:$H$98, 0))*Prices!$I$11*-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F108" s="2"/>
     </row>
   </sheetData>
@@ -11899,29 +11899,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.140625" customWidth="1"/>
-    <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" customWidth="1"/>
+    <col min="2" max="2" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.1796875" customWidth="1"/>
+    <col min="8" max="8" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C2" s="49" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1">
         <v>5000</v>
@@ -11931,12 +11931,12 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1">
         <v>5000</v>
@@ -11946,26 +11946,26 @@
       </c>
       <c r="E4" s="1"/>
       <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="E5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
         <v>37</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
       </c>
       <c r="I5" s="3">
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="43">
         <v>18000</v>
@@ -11977,15 +11977,15 @@
         <v>0.4</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="3">
         <v>0.45</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="43">
         <v>8100</v>
@@ -11997,30 +11997,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C8" s="44"/>
       <c r="D8" s="40"/>
       <c r="H8" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C9" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="45">
         <v>1200</v>
@@ -12029,13 +12029,13 @@
         <v>0.05</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="3">
         <v>0.45</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
@@ -12046,15 +12046,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="45">
         <v>2400</v>
@@ -12063,7 +12063,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="17" t="s">
         <v>12</v>
       </c>
@@ -12075,7 +12075,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="17" t="s">
         <v>13</v>
       </c>
@@ -12086,15 +12086,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H14" s="62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" s="61">
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="17" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C15" s="45">
         <v>4800</v>
@@ -12103,15 +12103,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I15" s="55">
         <v>43466</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="46">
         <v>12000</v>
@@ -12122,9 +12122,9 @@
       <c r="H16" s="4"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="46">
         <v>6000</v>
@@ -12133,9 +12133,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="46">
         <v>6000</v>
@@ -12144,13 +12144,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C19" s="44"/>
       <c r="D19" s="40"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="45">
         <v>10200</v>
@@ -12159,9 +12159,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="45">
         <v>39600</v>
@@ -12170,9 +12170,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="46">
         <v>42000</v>
@@ -12181,9 +12181,9 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="46">
         <v>33600</v>

</xml_diff>

<commit_message>
Update the HCG Benchmark distribution
Do this because it had summed to greater than 100%
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -1021,7 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -2184,11 +2184,11 @@
   </sheetPr>
   <dimension ref="B1:N62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N54" sqref="N54"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,19 +2274,19 @@
         <v>0</v>
       </c>
       <c r="K4" s="12">
-        <f>F4*$D4</f>
+        <f t="shared" ref="K4:N5" si="0">F4*$D4</f>
         <v>2500</v>
       </c>
       <c r="L4" s="12">
-        <f>G4*$D4</f>
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="M4" s="12">
-        <f>H4*$D4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4" s="12">
-        <f>I4*$D4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2313,19 +2313,19 @@
         <v>0</v>
       </c>
       <c r="K5" s="12">
-        <f>F5*$D5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="12">
-        <f>G5*$D5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M5" s="12">
-        <f>H5*$D5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N5" s="12">
-        <f>I5*$D5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2366,7 +2366,7 @@
         <v>0.6</v>
       </c>
       <c r="H8" s="35">
-        <f t="shared" ref="H8:H18" si="0">1-SUM(F8:G8)</f>
+        <f t="shared" ref="H8:H18" si="1">1-SUM(F8:G8)</f>
         <v>0</v>
       </c>
       <c r="I8" s="35">
@@ -2381,7 +2381,7 @@
         <v>10800</v>
       </c>
       <c r="M8" s="16">
-        <f t="shared" ref="M8:N18" si="1">H8*$D8</f>
+        <f t="shared" ref="M8:N18" si="2">H8*$D8</f>
         <v>0</v>
       </c>
       <c r="N8" s="16">
@@ -2405,26 +2405,26 @@
         <v>0.8</v>
       </c>
       <c r="H9" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" s="35">
         <v>0</v>
       </c>
       <c r="K9" s="16">
-        <f t="shared" ref="K9:K18" si="2">F9*$D9</f>
+        <f t="shared" ref="K9:K18" si="3">F9*$D9</f>
         <v>1620</v>
       </c>
       <c r="L9" s="16">
-        <f t="shared" ref="L9:L17" si="3">G9*$D9</f>
+        <f t="shared" ref="L9:L17" si="4">G9*$D9</f>
         <v>6480</v>
       </c>
       <c r="M9" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N9" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2444,26 +2444,26 @@
         <v>0.9</v>
       </c>
       <c r="H10" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="37">
         <v>0</v>
       </c>
       <c r="K10" s="18">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="L10" s="18">
+        <f t="shared" si="4"/>
+        <v>1080</v>
+      </c>
+      <c r="M10" s="18">
         <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="3"/>
-        <v>1080</v>
-      </c>
-      <c r="M10" s="18">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N10" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2489,19 +2489,19 @@
         <v>0.1</v>
       </c>
       <c r="K11" s="18">
-        <f t="shared" si="2"/>
-        <v>2160</v>
-      </c>
-      <c r="L11" s="18">
         <f t="shared" si="3"/>
         <v>2160</v>
       </c>
+      <c r="L11" s="18">
+        <f t="shared" si="4"/>
+        <v>2160</v>
+      </c>
       <c r="M11" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N11" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>480</v>
       </c>
     </row>
@@ -2520,26 +2520,26 @@
         <v>0.1</v>
       </c>
       <c r="H12" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I12" s="37">
         <v>0</v>
       </c>
       <c r="K12" s="18">
+        <f t="shared" si="3"/>
+        <v>2160</v>
+      </c>
+      <c r="L12" s="18">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="M12" s="18">
         <f t="shared" si="2"/>
-        <v>2160</v>
-      </c>
-      <c r="L12" s="18">
-        <f t="shared" si="3"/>
-        <v>240</v>
-      </c>
-      <c r="M12" s="18">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2558,26 +2558,26 @@
         <v>0.9</v>
       </c>
       <c r="H13" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I13" s="37">
         <v>0</v>
       </c>
       <c r="K13" s="18">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="L13" s="18">
+        <f t="shared" si="4"/>
+        <v>2160</v>
+      </c>
+      <c r="M13" s="18">
         <f t="shared" si="2"/>
-        <v>240</v>
-      </c>
-      <c r="L13" s="18">
-        <f t="shared" si="3"/>
-        <v>2160</v>
-      </c>
-      <c r="M13" s="18">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2602,15 +2602,15 @@
         <v>0</v>
       </c>
       <c r="K14" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="18">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N14" s="18">
@@ -2633,26 +2633,26 @@
         <v>0.4</v>
       </c>
       <c r="H15" s="37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I15" s="37">
         <v>0</v>
       </c>
       <c r="K15" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L15" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N15" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2671,26 +2671,26 @@
         <v>0.9</v>
       </c>
       <c r="H16" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I16" s="38">
         <v>0</v>
       </c>
       <c r="K16" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L16" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N16" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2709,26 +2709,26 @@
         <v>0.9</v>
       </c>
       <c r="H17" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I17" s="38">
         <v>0</v>
       </c>
       <c r="K17" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L17" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N17" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2747,14 +2747,14 @@
         <v>0.9</v>
       </c>
       <c r="H18" s="38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I18" s="38">
         <v>0</v>
       </c>
       <c r="K18" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L18" s="20">
@@ -2762,11 +2762,11 @@
         <v>0</v>
       </c>
       <c r="M18" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N18" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2826,7 +2826,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="G23" s="35">
-        <f t="shared" ref="G23:G33" si="4">MIN(1,G8+$H$20)</f>
+        <f t="shared" ref="G23:G33" si="5">MIN(1,G8+$H$20)</f>
         <v>0.7</v>
       </c>
       <c r="H23" s="35">
@@ -2842,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="16">
-        <f t="shared" ref="L23:L33" si="5">G23*$D23</f>
+        <f t="shared" ref="L23:L33" si="6">G23*$D23</f>
         <v>0</v>
       </c>
       <c r="M23" s="16">
@@ -2864,35 +2864,35 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="36">
-        <f t="shared" ref="F24:F33" si="6">(1-G24)*F9/SUM(F9,H9)</f>
+        <f t="shared" ref="F24:F33" si="7">(1-G24)*F9/SUM(F9,H9)</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="G24" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="H24" s="36">
-        <f t="shared" ref="H24:H33" si="7">IF(H9=0, 0,(1-G24)*H9/SUM(F9,H9))</f>
+        <f t="shared" ref="H24:H33" si="8">IF(H9=0, 0,(1-G24)*H9/SUM(F9,H9))</f>
         <v>0</v>
       </c>
       <c r="I24" s="36">
-        <f t="shared" ref="I24:I33" si="8">IF(I9=0, 0,(1-G24)*I9/SUM(F9,I9))</f>
+        <f t="shared" ref="I24:I33" si="9">IF(I9=0, 0,(1-G24)*I9/SUM(F9,I9))</f>
         <v>0</v>
       </c>
       <c r="K24" s="29">
-        <f t="shared" ref="K24:K33" si="9">F24*$D24</f>
+        <f t="shared" ref="K24:K33" si="10">F24*$D24</f>
         <v>0</v>
       </c>
       <c r="L24" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M24" s="29">
-        <f t="shared" ref="M23:N33" si="10">H24*$D24</f>
+        <f t="shared" ref="M24:N33" si="11">H24*$D24</f>
         <v>0</v>
       </c>
       <c r="N24" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -2906,35 +2906,35 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H25" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="37">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="18">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G25" s="37">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="H25" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="18">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="M25" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N25" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -2948,35 +2948,35 @@
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="37">
+        <f>(1-G26)*F11/SUM(F11,H11, I11)</f>
+        <v>0.36818181818181811</v>
+      </c>
+      <c r="G26" s="37">
+        <f t="shared" si="5"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H26" s="37">
+        <f>IF(H11=0, 0,(1-G26)*H11/SUM(F11,H11))</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="37">
+        <f t="shared" si="9"/>
+        <v>8.1818181818181804E-2</v>
+      </c>
+      <c r="K26" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="18">
         <f t="shared" si="6"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G26" s="37">
-        <f t="shared" si="4"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H26" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="37">
-        <f t="shared" si="8"/>
-        <v>8.1818181818181804E-2</v>
-      </c>
-      <c r="K26" s="18">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M26" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N26" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -2989,35 +2989,35 @@
         <v>0</v>
       </c>
       <c r="F27" s="37">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+      <c r="G27" s="37">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="H27" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="37">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="18">
         <f t="shared" si="6"/>
-        <v>0.8</v>
-      </c>
-      <c r="G27" s="37">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
-      </c>
-      <c r="H27" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="18">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="18">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M27" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N27" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3030,35 +3030,35 @@
         <v>0</v>
       </c>
       <c r="F28" s="37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H28" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="37">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="18">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G28" s="37">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="H28" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="18">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="M28" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N28" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3071,35 +3071,35 @@
         <v>0</v>
       </c>
       <c r="F29" s="37">
+        <f t="shared" si="7"/>
+        <v>8.8888888888888906E-2</v>
+      </c>
+      <c r="G29" s="37">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="H29" s="37">
+        <f t="shared" si="8"/>
+        <v>0.71111111111111125</v>
+      </c>
+      <c r="I29" s="37">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="18">
         <f t="shared" si="6"/>
-        <v>8.8888888888888906E-2</v>
-      </c>
-      <c r="G29" s="37">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
-      </c>
-      <c r="H29" s="37">
-        <f t="shared" si="7"/>
-        <v>0.71111111111111125</v>
-      </c>
-      <c r="I29" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="18">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="18">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M29" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N29" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3112,35 +3112,35 @@
         <v>0</v>
       </c>
       <c r="F30" s="37">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="37">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="37">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="18">
         <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="G30" s="37">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="H30" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="37">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="18">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="18">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M30" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N30" s="18">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3153,35 +3153,35 @@
         <v>0</v>
       </c>
       <c r="F31" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H31" s="38">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G31" s="38">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="H31" s="38">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="38">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L31" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="M31" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N31" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3194,35 +3194,35 @@
         <v>0</v>
       </c>
       <c r="F32" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H32" s="38">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G32" s="38">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="H32" s="38">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="38">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L32" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="M32" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N32" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3235,35 +3235,35 @@
         <v>0</v>
       </c>
       <c r="F33" s="36">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="36">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="36">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="36">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="29">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="29">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G33" s="36">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="H33" s="36">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="29">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="29">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="M33" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N33" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3310,19 +3310,19 @@
         <v>0</v>
       </c>
       <c r="K36" s="18">
-        <f>F36*$D36</f>
+        <f t="shared" ref="K36:N39" si="12">F36*$D36</f>
         <v>9180</v>
       </c>
       <c r="L36" s="18">
-        <f>G36*$D36</f>
+        <f t="shared" si="12"/>
         <v>1020</v>
       </c>
       <c r="M36" s="18">
-        <f>H36*$D36</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N36" s="18">
-        <f>I36*$D36</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -3348,19 +3348,19 @@
         <v>0</v>
       </c>
       <c r="K37" s="18">
-        <f>F37*$D37</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L37" s="18">
-        <f>G37*$D37</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M37" s="18">
-        <f>H37*$D37</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N37" s="18">
-        <f>I37*$D37</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -3379,26 +3379,26 @@
         <v>0.9</v>
       </c>
       <c r="H38" s="38">
-        <f t="shared" ref="H38:H39" si="11">1-SUM(F38:G38)</f>
+        <f t="shared" ref="H38:H39" si="13">1-SUM(F38:G38)</f>
         <v>0</v>
       </c>
       <c r="I38" s="38">
         <v>0</v>
       </c>
       <c r="K38" s="20">
-        <f>F38*$D38</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L38" s="20">
-        <f>G38*$D38</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M38" s="20">
-        <f>H38*$D38</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N38" s="20">
-        <f>I38*$D38</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -3417,26 +3417,26 @@
         <v>0.9</v>
       </c>
       <c r="H39" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I39" s="38">
         <v>0</v>
       </c>
       <c r="K39" s="20">
-        <f>F39*$D39</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L39" s="20">
-        <f>G39*$D39</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M39" s="20">
-        <f>H39*$D39</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N39" s="20">
-        <f>I39*$D39</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="29">
-        <f t="shared" ref="L42:L45" si="12">G42*$D42</f>
+        <f t="shared" ref="L42:L45" si="14">G42*$D42</f>
         <v>0</v>
       </c>
       <c r="M42" s="29">
@@ -3525,15 +3525,15 @@
         <v>0</v>
       </c>
       <c r="L43" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M43" s="18">
-        <f t="shared" ref="M42:N45" si="13">H43*$D43</f>
+        <f t="shared" ref="M43:N45" si="15">H43*$D43</f>
         <v>0</v>
       </c>
       <c r="N43" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3561,19 +3561,19 @@
         <v>0</v>
       </c>
       <c r="K44" s="20">
-        <f t="shared" ref="K44:K45" si="14">F44*$D44</f>
+        <f t="shared" ref="K44:K45" si="16">F44*$D44</f>
         <v>0</v>
       </c>
       <c r="L44" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M44" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N44" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3590,7 +3590,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="31">
-        <f t="shared" ref="G43:G45" si="15">MIN(1,G39+$H$20)</f>
+        <f t="shared" ref="G45" si="17">MIN(1,G39+$H$20)</f>
         <v>1</v>
       </c>
       <c r="H45" s="31">
@@ -3601,19 +3601,19 @@
         <v>0</v>
       </c>
       <c r="K45" s="20">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="20">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="L45" s="20">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
       <c r="M45" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N45" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3730,7 +3730,7 @@
         <v>22680</v>
       </c>
       <c r="L51" s="12">
-        <f t="shared" ref="L51:M51" si="16">SUM(L48:L49, L36:L39, L8:L18,L23:L33,L42:L45)</f>
+        <f t="shared" ref="L51" si="18">SUM(L48:L49, L36:L39, L8:L18,L23:L33,L42:L45)</f>
         <v>23940</v>
       </c>
       <c r="M51" s="12">
@@ -3852,19 +3852,19 @@
       </c>
       <c r="J59" s="21"/>
       <c r="K59" s="25">
-        <f>F59*$D59</f>
+        <f t="shared" ref="K59:N62" si="19">F59*$D59</f>
         <v>9180</v>
       </c>
       <c r="L59" s="25">
-        <f>G59*$D59</f>
+        <f t="shared" si="19"/>
         <v>1020</v>
       </c>
       <c r="M59" s="25">
-        <f>H59*$D59</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N59" s="25">
-        <f>I59*$D59</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
         <v>0.45348837209302323</v>
       </c>
       <c r="G60" s="24">
-        <f t="shared" ref="G60:H60" si="17">IFERROR(SUM(L$37,L$10:L$15,L$43,L$25:L$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
+        <f t="shared" ref="G60" si="20">IFERROR(SUM(L$37,L$10:L$15,L$43,L$25:L$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
         <v>0.54651162790697672</v>
       </c>
       <c r="H60" s="24">
@@ -3896,19 +3896,19 @@
       </c>
       <c r="J60" s="21"/>
       <c r="K60" s="25">
-        <f>F60*$D60</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L60" s="25">
-        <f>G60*$D60</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M60" s="25">
-        <f>H60*$D60</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N60" s="25">
-        <f>I60*$D60</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -3940,19 +3940,19 @@
       </c>
       <c r="J61" s="21"/>
       <c r="K61" s="25">
-        <f>F61*$D61</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L61" s="25">
-        <f>G61*$D61</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M61" s="25">
-        <f>H61*$D61</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N61" s="25">
-        <f>I61*$D61</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -3984,19 +3984,19 @@
       </c>
       <c r="J62" s="21"/>
       <c r="K62" s="25">
-        <f>F62*$D62</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L62" s="25">
-        <f>G62*$D62</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M62" s="25">
-        <f>H62*$D62</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="N62" s="25">
-        <f>I62*$D62</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix calcs for PRM products
Do this because the PMPM forces needed to reference a different input
row for PRM add-ons than ACOI add-ons
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
+++ b/0273NYP - New York Premier/Monthly_Premier_Pricing_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shea.parkes\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason.Altieri\repos\client-and-project-documentation\0273NYP - New York Premier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890" activeTab="4"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="13680" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -1075,11 +1075,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="56">
-        <v>750000</v>
+        <v>250000</v>
       </c>
       <c r="E7" s="56"/>
       <c r="F7" s="56"/>
@@ -1375,7 +1375,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="D7" s="16">
         <f>SUM(Calcs!D40, Calcs!D53)</f>
-        <v>109400</v>
+        <v>69400</v>
       </c>
       <c r="E7" s="16">
         <f>SUM(Calcs!E40, Calcs!E53)</f>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="D21" s="1">
         <f>SUM(Calcs!D67, Calcs!D73)</f>
-        <v>116000</v>
+        <v>76000</v>
       </c>
       <c r="E21" s="1">
         <f>SUM(Calcs!E67, Calcs!E73)</f>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="D30" s="7">
         <f>SUM(D7:D17, D20:D23, D26:D28)</f>
-        <v>233500</v>
+        <v>153500</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" ref="E30:H30" si="0">SUM(E7:E17, E20:E23, E26:E27)</f>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D35" s="7">
         <f>(D30/12*Inputs!$C$2+D4)*$C$33</f>
-        <v>733250</v>
+        <v>493250</v>
       </c>
       <c r="E35" s="7">
         <f>(E30/12*Inputs!$C$2+E4)*$C$33</f>
@@ -2231,13 +2231,13 @@
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" s="7">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>733250</v>
+        <v>493250</v>
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" s="53">
         <f>SUM(D35:H35)</f>
-        <v>733250</v>
+        <v>493250</v>
       </c>
       <c r="D40" s="1"/>
       <c r="G40" s="1"/>
@@ -2270,10 +2270,10 @@
   <dimension ref="B1:N63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G58" sqref="G58"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,7 +2288,7 @@
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.85546875" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="D23" s="16">
         <f>SUM(Calcs!D27:H27)</f>
-        <v>76400</v>
+        <v>36400</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="35">
@@ -2924,11 +2924,11 @@
       </c>
       <c r="K23" s="16">
         <f>F23*$D23</f>
-        <v>22920.000000000004</v>
+        <v>10920.000000000002</v>
       </c>
       <c r="L23" s="16">
         <f t="shared" ref="L23:L33" si="6">G23*$D23</f>
-        <v>53480</v>
+        <v>25480</v>
       </c>
       <c r="M23" s="16">
         <f>H23*$D23</f>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="D25" s="18">
         <f>SUM(Calcs!D29:H29)</f>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="37">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="L25" s="18">
         <f t="shared" si="6"/>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="M25" s="18">
         <f t="shared" si="11"/>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="D26" s="18">
         <f>SUM(Calcs!D30:H30)</f>
-        <v>13370.000000000002</v>
+        <v>6370.0000000000009</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="37">
@@ -3050,11 +3050,11 @@
       </c>
       <c r="K26" s="18">
         <f t="shared" si="10"/>
-        <v>4922.590909090909</v>
+        <v>2345.3181818181815</v>
       </c>
       <c r="L26" s="18">
         <f t="shared" si="6"/>
-        <v>7353.5000000000018</v>
+        <v>3503.5000000000009</v>
       </c>
       <c r="M26" s="18">
         <f t="shared" si="11"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="N26" s="18">
         <f t="shared" si="11"/>
-        <v>1093.9090909090908</v>
+        <v>521.18181818181813</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="D27" s="18">
         <f>SUM(Calcs!D31:H31)</f>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="F27" s="37">
         <f t="shared" si="7"/>
@@ -3091,11 +3091,11 @@
       </c>
       <c r="K27" s="18">
         <f t="shared" si="10"/>
-        <v>7640</v>
+        <v>3640</v>
       </c>
       <c r="L27" s="18">
         <f t="shared" si="6"/>
-        <v>1910</v>
+        <v>910</v>
       </c>
       <c r="M27" s="18">
         <f t="shared" si="11"/>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="D28" s="18">
         <f>SUM(Calcs!D32:H32)</f>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="F28" s="37">
         <f t="shared" si="7"/>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="L28" s="18">
         <f t="shared" si="6"/>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="M28" s="18">
         <f t="shared" si="11"/>
@@ -3153,7 +3153,7 @@
       </c>
       <c r="D29" s="18">
         <f>SUM(Calcs!D33:H33)</f>
-        <v>13370.000000000002</v>
+        <v>6370.0000000000009</v>
       </c>
       <c r="F29" s="37">
         <f t="shared" si="7"/>
@@ -3173,15 +3173,15 @@
       </c>
       <c r="K29" s="18">
         <f t="shared" si="10"/>
-        <v>1188.4444444444448</v>
+        <v>566.2222222222224</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" si="6"/>
-        <v>2674.0000000000005</v>
+        <v>1274.0000000000002</v>
       </c>
       <c r="M29" s="18">
         <f t="shared" si="11"/>
-        <v>9507.5555555555584</v>
+        <v>4529.7777777777792</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" si="11"/>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="D30" s="18">
         <f>SUM(Calcs!D34:H34)</f>
-        <v>13370.000000000002</v>
+        <v>6370.0000000000009</v>
       </c>
       <c r="F30" s="37">
         <f t="shared" si="7"/>
@@ -3214,11 +3214,11 @@
       </c>
       <c r="K30" s="18">
         <f t="shared" si="10"/>
-        <v>6685.0000000000009</v>
+        <v>3185.0000000000005</v>
       </c>
       <c r="L30" s="18">
         <f t="shared" si="6"/>
-        <v>6685.0000000000009</v>
+        <v>3185.0000000000005</v>
       </c>
       <c r="M30" s="18">
         <f t="shared" si="11"/>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="D31" s="20">
         <f>SUM(Calcs!D35:H35)</f>
-        <v>47750</v>
+        <v>0</v>
       </c>
       <c r="F31" s="38">
         <f t="shared" si="7"/>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="L31" s="20">
         <f t="shared" si="6"/>
-        <v>47750</v>
+        <v>0</v>
       </c>
       <c r="M31" s="20">
         <f t="shared" si="11"/>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="D32" s="20">
         <f>SUM(Calcs!D36:H36)</f>
-        <v>19100</v>
+        <v>0</v>
       </c>
       <c r="F32" s="38">
         <f t="shared" si="7"/>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="L32" s="20">
         <f t="shared" si="6"/>
-        <v>19100</v>
+        <v>0</v>
       </c>
       <c r="M32" s="20">
         <f t="shared" si="11"/>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="D43" s="18">
         <f>SUM(Calcs!D85:H85)</f>
-        <v>7640</v>
+        <v>3640</v>
       </c>
       <c r="F43" s="30">
         <f>IFERROR((1-G43)*F37/SUM(F37,H37),0)</f>
@@ -3607,11 +3607,11 @@
       </c>
       <c r="K43" s="18">
         <f>F43*$D43</f>
-        <v>6112</v>
+        <v>2912</v>
       </c>
       <c r="L43" s="18">
         <f t="shared" si="14"/>
-        <v>1528</v>
+        <v>728</v>
       </c>
       <c r="M43" s="18">
         <f t="shared" ref="M43:N45" si="15">H43*$D43</f>
@@ -3725,19 +3725,19 @@
       </c>
       <c r="F48" s="8">
         <f>IFERROR(SUM(K60:K63)/SUM($K$60:$M$63), 0)</f>
-        <v>0.43730082116538704</v>
+        <v>0.48152508107883424</v>
       </c>
       <c r="G48" s="8">
         <f>IFERROR(SUM(L60:L63)/SUM($K$60:$M$63), 0)</f>
-        <v>0.43084361392076442</v>
+        <v>0.38283795769753576</v>
       </c>
       <c r="H48" s="8">
         <f>IFERROR(SUM(M60:M63)/SUM($K$60:$M$63), 0)</f>
-        <v>0.13185556491384848</v>
+        <v>0.13563696122362989</v>
       </c>
       <c r="I48" s="8">
         <f>IFERROR(SUM(N60:N63)/SUM($K$60:$M$63), 0)</f>
-        <v>1.3592789726535125E-2</v>
+        <v>1.3197297588272877E-2</v>
       </c>
       <c r="K48" s="12">
         <f>F48*$D$48</f>
@@ -3766,19 +3766,19 @@
       </c>
       <c r="F49" s="3">
         <f>IFERROR(SUM(K8:K48)/SUM($K8:$N48), 0)</f>
-        <v>0.29195283953233014</v>
+        <v>0.40253120784391144</v>
       </c>
       <c r="G49" s="3">
         <f>IFERROR(SUM(L8:L48)/SUM($K8:$N48), 0)</f>
-        <v>0.65197436324288327</v>
+        <v>0.52391205211726388</v>
       </c>
       <c r="H49" s="3">
         <f>IFERROR(SUM(M8:M48)/SUM($K8:$N48), 0)</f>
-        <v>5.0832547213436184E-2</v>
+        <v>6.7034382917119079E-2</v>
       </c>
       <c r="I49" s="3">
         <f>1-F49-G49-H49</f>
-        <v>5.2402500113504571E-3</v>
+        <v>6.522357121705652E-3</v>
       </c>
       <c r="K49" s="12">
         <f>F49*$D$49</f>
@@ -3846,23 +3846,23 @@
       </c>
       <c r="D52" s="1">
         <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
-        <v>233500</v>
+        <v>153500</v>
       </c>
       <c r="K52" s="12">
         <f>SUM(K48:K50, K36:K39, K8:K18,K23:K33,K42:K45)</f>
-        <v>87688.03535353535</v>
+        <v>61788.540404040403</v>
       </c>
       <c r="L52" s="12">
-        <f t="shared" ref="L52:N52" si="19">SUM(L48:L50, L36:L39, L8:L18,L23:L33,L42:L45)</f>
-        <v>195820.5</v>
+        <f>SUM(L48:L50, L36:L39, L8:L18,L23:L33,L42:L45)</f>
+        <v>80420.5</v>
       </c>
       <c r="M52" s="12">
-        <f t="shared" si="19"/>
-        <v>15267.555555555558</v>
+        <f t="shared" ref="L52:N52" si="19">SUM(M48:M50, M36:M39, M8:M18,M23:M33,M42:M45)</f>
+        <v>10289.777777777779</v>
       </c>
       <c r="N52" s="12">
         <f t="shared" si="19"/>
-        <v>1573.9090909090908</v>
+        <v>1001.1818181818181</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="D53" s="23">
         <f>SUM(K52:N52)</f>
-        <v>300350</v>
+        <v>153500</v>
       </c>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
@@ -3888,42 +3888,42 @@
       </c>
       <c r="D55" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>733250</v>
+        <v>493250</v>
       </c>
       <c r="K55" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>266339.10606060602</v>
+        <v>188640.62121212113</v>
       </c>
       <c r="L55" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
-        <v>616936.5</v>
+        <v>270736.5</v>
       </c>
       <c r="M55" s="12">
         <f>SUM(Outputs_Timeline!V:V)</f>
-        <v>45802.666666666679</v>
+        <v>30869.333333333339</v>
       </c>
       <c r="N55" s="12">
         <f>SUM(Outputs_Timeline!W:W)</f>
-        <v>4721.7272727272739</v>
+        <v>3003.545454545454</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="K56" s="54">
         <f>IFERROR(K55/$D$55, 0)</f>
-        <v>0.36323096632881829</v>
+        <v>0.38244423965964752</v>
       </c>
       <c r="L56" s="54">
         <f>IFERROR(L55/$D$55, 0)</f>
-        <v>0.84137265598363453</v>
+        <v>0.5488829194120628</v>
       </c>
       <c r="M56" s="54">
         <f>IFERROR(M55/$D$55, 0)</f>
-        <v>6.2465280145471092E-2</v>
+        <v>6.2583544517655021E-2</v>
       </c>
       <c r="N56" s="54">
         <f>IFERROR(N55/$D$55, 0)</f>
-        <v>6.4394507640331044E-3</v>
+        <v>6.0892964106344736E-3</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -3998,41 +3998,41 @@
       </c>
       <c r="D61" s="23">
         <f>SUM(Calcs!D67:H67)+SUM(Calcs!D73:H73)</f>
-        <v>116000</v>
+        <v>76000</v>
       </c>
       <c r="E61" s="21"/>
       <c r="F61" s="24">
         <f>IFERROR(SUM(K$37,K$10:K$15,K$43,K$25:K$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
-        <v>0.43650914714213218</v>
+        <v>0.48065477934130413</v>
       </c>
       <c r="G61" s="24">
         <f t="shared" ref="G61" si="21">IFERROR(SUM(L$37,L$10:L$15,L$43,L$25:L$30)/SUM($K$37:$M$37,$K$10:$M$15,$K$43:$M$43,$K$25:$M$30),0)</f>
-        <v>0.43006362979835333</v>
+        <v>0.38214602169488732</v>
       </c>
       <c r="H61" s="24">
         <f>IFERROR(SUM(M$37,M$10:M$15,M$43,M$25:M$30)/SUM($K$37:$N$37,$K$10:$N$15,$K$43:$N$43,$K$25:$N$30),0)</f>
-        <v>0.13161685823754793</v>
+        <v>0.13539181286549709</v>
       </c>
       <c r="I61" s="24">
         <f>IFERROR(SUM(N$37,N$10:N$15,N$43,N$25:N$30)/SUM($K$37:$N$37,$K$10:$N$15,$K$43:$N$43,$K$25:$N$30),0)</f>
-        <v>1.3568181818181818E-2</v>
+        <v>1.3173444976076554E-2</v>
       </c>
       <c r="J61" s="21"/>
       <c r="K61" s="25">
         <f t="shared" si="20"/>
-        <v>50635.061068487332</v>
+        <v>36529.763229939112</v>
       </c>
       <c r="L61" s="25">
         <f t="shared" si="20"/>
-        <v>49887.381056608989</v>
+        <v>29043.097648811436</v>
       </c>
       <c r="M61" s="25">
         <f t="shared" si="20"/>
-        <v>15267.55555555556</v>
+        <v>10289.777777777779</v>
       </c>
       <c r="N61" s="25">
         <f t="shared" si="20"/>
-        <v>1573.9090909090908</v>
+        <v>1001.1818181818181</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -4051,7 +4051,7 @@
       </c>
       <c r="G62" s="24">
         <f>IFERROR(SUM(L38,L16:L18,L44,L31:L33)/SUM($K$38:$M$38,$K$16:$M$18,$K$44:$M$44,$K$31:$M$33),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" s="24">
         <f>IFERROR(SUM(M38,M16:M18,M44,M31:M33)/SUM($K$38:$N$38,$K$16:$N$18,$K$44:$N$44,$K$31:$N$33),0)</f>
@@ -4684,23 +4684,23 @@
       </c>
       <c r="M9" s="67">
         <f>$F9*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N9" s="67">
         <f>$F9*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O9" s="67">
         <f>$F9*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P9" s="67">
         <f>$F9*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q9" s="67">
         <f>$F9*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S9" s="67">
         <f t="shared" si="1"/>
@@ -4758,23 +4758,23 @@
       </c>
       <c r="M10" s="67">
         <f>$F10*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N10" s="67">
         <f>$F10*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O10" s="67">
         <f>$F10*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P10" s="67">
         <f>$F10*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q10" s="67">
         <f>$F10*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S10" s="67">
         <f t="shared" si="1"/>
@@ -4832,43 +4832,43 @@
       </c>
       <c r="M11" s="67">
         <f>$F11*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N11" s="67">
         <f>$F11*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O11" s="67">
         <f>$F11*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P11" s="67">
         <f>$F11*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q11" s="67">
         <f>$F11*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S11" s="67">
         <f t="shared" si="1"/>
-        <v>91124.999999999985</v>
+        <v>71125</v>
       </c>
       <c r="T11" s="67">
         <f t="shared" si="2"/>
-        <v>25197.008838383841</v>
+        <v>18722.135101010103</v>
       </c>
       <c r="U11" s="67">
         <f>IF(MOD(MONTH($B11),3)=0,SUM(J9:J11,O9:O11),0)</f>
-        <v>78430.125</v>
+        <v>49580.125000000007</v>
       </c>
       <c r="V11" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W11" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
@@ -4906,23 +4906,23 @@
       </c>
       <c r="M12" s="67">
         <f>$F12*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N12" s="67">
         <f>$F12*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O12" s="67">
         <f>$F12*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P12" s="67">
         <f>$F12*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q12" s="67">
         <f>$F12*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S12" s="67">
         <f t="shared" si="1"/>
@@ -4980,23 +4980,23 @@
       </c>
       <c r="M13" s="67">
         <f>$F13*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N13" s="67">
         <f>$F13*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O13" s="67">
         <f>$F13*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P13" s="67">
         <f>$F13*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q13" s="67">
         <f>$F13*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S13" s="67">
         <f t="shared" si="1"/>
@@ -5054,43 +5054,43 @@
       </c>
       <c r="M14" s="67">
         <f>$F14*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N14" s="67">
         <f>$F14*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O14" s="67">
         <f>$F14*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P14" s="67">
         <f>$F14*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q14" s="67">
         <f>$F14*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S14" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T14" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U14" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V14" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W14" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
@@ -5128,23 +5128,23 @@
       </c>
       <c r="M15" s="67">
         <f>$F15*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N15" s="67">
         <f>$F15*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O15" s="67">
         <f>$F15*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P15" s="67">
         <f>$F15*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q15" s="67">
         <f>$F15*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S15" s="67">
         <f t="shared" si="1"/>
@@ -5202,23 +5202,23 @@
       </c>
       <c r="M16" s="67">
         <f>$F16*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N16" s="67">
         <f>$F16*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O16" s="67">
         <f>$F16*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P16" s="67">
         <f>$F16*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q16" s="67">
         <f>$F16*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S16" s="67">
         <f t="shared" si="1"/>
@@ -5276,43 +5276,43 @@
       </c>
       <c r="M17" s="67">
         <f>$F17*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N17" s="67">
         <f>$F17*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O17" s="67">
         <f>$F17*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P17" s="67">
         <f>$F17*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q17" s="67">
         <f>$F17*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S17" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T17" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U17" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V17" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W17" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
@@ -5350,23 +5350,23 @@
       </c>
       <c r="M18" s="67">
         <f>$F18*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N18" s="67">
         <f>$F18*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O18" s="67">
         <f>$F18*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P18" s="67">
         <f>$F18*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q18" s="67">
         <f>$F18*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S18" s="67">
         <f t="shared" si="1"/>
@@ -5424,23 +5424,23 @@
       </c>
       <c r="M19" s="67">
         <f>$F19*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N19" s="67">
         <f>$F19*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O19" s="67">
         <f>$F19*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P19" s="67">
         <f>$F19*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q19" s="67">
         <f>$F19*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S19" s="67">
         <f t="shared" si="1"/>
@@ -5498,43 +5498,43 @@
       </c>
       <c r="M20" s="67">
         <f>$F20*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N20" s="67">
         <f>$F20*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O20" s="67">
         <f>$F20*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P20" s="67">
         <f>$F20*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q20" s="67">
         <f>$F20*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S20" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T20" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U20" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V20" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W20" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
@@ -5572,23 +5572,23 @@
       </c>
       <c r="M21" s="67">
         <f>$F21*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N21" s="67">
         <f>$F21*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O21" s="67">
         <f>$F21*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P21" s="67">
         <f>$F21*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q21" s="67">
         <f>$F21*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S21" s="67">
         <f t="shared" si="1"/>
@@ -5646,23 +5646,23 @@
       </c>
       <c r="M22" s="67">
         <f>$F22*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N22" s="67">
         <f>$F22*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O22" s="67">
         <f>$F22*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P22" s="67">
         <f>$F22*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q22" s="67">
         <f>$F22*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S22" s="67">
         <f t="shared" si="1"/>
@@ -5720,43 +5720,43 @@
       </c>
       <c r="M23" s="67">
         <f>$F23*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N23" s="67">
         <f>$F23*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O23" s="67">
         <f>$F23*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P23" s="67">
         <f>$F23*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q23" s="67">
         <f>$F23*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S23" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T23" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U23" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V23" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W23" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
@@ -5794,23 +5794,23 @@
       </c>
       <c r="M24" s="67">
         <f>$F24*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N24" s="67">
         <f>$F24*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O24" s="67">
         <f>$F24*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P24" s="67">
         <f>$F24*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q24" s="67">
         <f>$F24*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S24" s="67">
         <f t="shared" si="1"/>
@@ -5868,23 +5868,23 @@
       </c>
       <c r="M25" s="67">
         <f>$F25*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N25" s="67">
         <f>$F25*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O25" s="67">
         <f>$F25*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P25" s="67">
         <f>$F25*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q25" s="67">
         <f>$F25*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S25" s="67">
         <f t="shared" si="1"/>
@@ -5942,43 +5942,43 @@
       </c>
       <c r="M26" s="67">
         <f>$F26*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N26" s="67">
         <f>$F26*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O26" s="67">
         <f>$F26*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P26" s="67">
         <f>$F26*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q26" s="67">
         <f>$F26*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S26" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T26" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U26" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V26" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W26" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
@@ -6016,23 +6016,23 @@
       </c>
       <c r="M27" s="67">
         <f>$F27*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N27" s="67">
         <f>$F27*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O27" s="67">
         <f>$F27*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P27" s="67">
         <f>$F27*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q27" s="67">
         <f>$F27*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S27" s="67">
         <f t="shared" si="1"/>
@@ -6090,23 +6090,23 @@
       </c>
       <c r="M28" s="67">
         <f>$F28*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N28" s="67">
         <f>$F28*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O28" s="67">
         <f>$F28*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P28" s="67">
         <f>$F28*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q28" s="67">
         <f>$F28*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S28" s="67">
         <f t="shared" si="1"/>
@@ -6164,43 +6164,43 @@
       </c>
       <c r="M29" s="67">
         <f>$F29*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N29" s="67">
         <f>$F29*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O29" s="67">
         <f>$F29*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P29" s="67">
         <f>$F29*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q29" s="67">
         <f>$F29*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S29" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T29" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U29" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V29" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W29" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
@@ -6238,23 +6238,23 @@
       </c>
       <c r="M30" s="67">
         <f>$F30*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N30" s="67">
         <f>$F30*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O30" s="67">
         <f>$F30*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P30" s="67">
         <f>$F30*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q30" s="67">
         <f>$F30*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S30" s="67">
         <f t="shared" si="1"/>
@@ -6312,23 +6312,23 @@
       </c>
       <c r="M31" s="67">
         <f>$F31*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N31" s="67">
         <f>$F31*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O31" s="67">
         <f>$F31*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P31" s="67">
         <f>$F31*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q31" s="67">
         <f>$F31*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S31" s="67">
         <f t="shared" si="1"/>
@@ -6386,43 +6386,43 @@
       </c>
       <c r="M32" s="67">
         <f>$F32*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N32" s="67">
         <f>$F32*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O32" s="67">
         <f>$F32*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P32" s="67">
         <f>$F32*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q32" s="67">
         <f>$F32*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S32" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T32" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U32" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V32" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W32" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
@@ -6460,23 +6460,23 @@
       </c>
       <c r="M33" s="67">
         <f>$F33*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N33" s="67">
         <f>$F33*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O33" s="67">
         <f>$F33*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P33" s="67">
         <f>$F33*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q33" s="67">
         <f>$F33*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S33" s="67">
         <f t="shared" si="1"/>
@@ -6534,23 +6534,23 @@
       </c>
       <c r="M34" s="67">
         <f>$F34*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N34" s="67">
         <f>$F34*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O34" s="67">
         <f>$F34*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P34" s="67">
         <f>$F34*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q34" s="67">
         <f>$F34*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S34" s="67">
         <f t="shared" si="1"/>
@@ -6608,43 +6608,43 @@
       </c>
       <c r="M35" s="67">
         <f>$F35*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N35" s="67">
         <f>$F35*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O35" s="67">
         <f>$F35*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P35" s="67">
         <f>$F35*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q35" s="67">
         <f>$F35*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S35" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T35" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U35" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V35" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W35" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
@@ -6682,23 +6682,23 @@
       </c>
       <c r="M36" s="67">
         <f>$F36*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N36" s="67">
         <f>$F36*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O36" s="67">
         <f>$F36*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P36" s="67">
         <f>$F36*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q36" s="67">
         <f>$F36*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S36" s="67">
         <f t="shared" si="1"/>
@@ -6756,23 +6756,23 @@
       </c>
       <c r="M37" s="67">
         <f>$F37*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N37" s="67">
         <f>$F37*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O37" s="67">
         <f>$F37*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P37" s="67">
         <f>$F37*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q37" s="67">
         <f>$F37*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S37" s="67">
         <f t="shared" si="1"/>
@@ -6830,43 +6830,43 @@
       </c>
       <c r="M38" s="67">
         <f>$F38*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N38" s="67">
         <f>$F38*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O38" s="67">
         <f>$F38*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P38" s="67">
         <f>$F38*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q38" s="67">
         <f>$F38*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S38" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T38" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U38" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V38" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W38" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
@@ -6904,23 +6904,23 @@
       </c>
       <c r="M39" s="67">
         <f>$F39*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N39" s="67">
         <f>$F39*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O39" s="67">
         <f>$F39*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P39" s="67">
         <f>$F39*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q39" s="67">
         <f>$F39*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S39" s="67">
         <f t="shared" si="1"/>
@@ -6978,23 +6978,23 @@
       </c>
       <c r="M40" s="67">
         <f>$F40*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N40" s="67">
         <f>$F40*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O40" s="67">
         <f>$F40*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P40" s="67">
         <f>$F40*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q40" s="67">
         <f>$F40*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S40" s="67">
         <f t="shared" si="1"/>
@@ -7052,43 +7052,43 @@
       </c>
       <c r="M41" s="67">
         <f>$F41*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N41" s="67">
         <f>$F41*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O41" s="67">
         <f>$F41*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P41" s="67">
         <f>$F41*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q41" s="67">
         <f>$F41*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S41" s="67">
         <f t="shared" si="1"/>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T41" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U41" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V41" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W41" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
@@ -7126,23 +7126,23 @@
       </c>
       <c r="M42" s="67">
         <f>$F42*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N42" s="67">
         <f>$F42*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O42" s="67">
         <f>$F42*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P42" s="67">
         <f>$F42*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q42" s="67">
         <f>$F42*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S42" s="67">
         <f t="shared" si="1"/>
@@ -7200,23 +7200,23 @@
       </c>
       <c r="M43" s="67">
         <f>$F43*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N43" s="67">
         <f>$F43*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O43" s="67">
         <f>$F43*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P43" s="67">
         <f>$F43*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q43" s="67">
         <f>$F43*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S43" s="67">
         <f t="shared" si="1"/>
@@ -7274,43 +7274,43 @@
       </c>
       <c r="M44" s="67">
         <f>$F44*Outputs_Internal!$D$52/12</f>
-        <v>19458.333333333332</v>
+        <v>12791.666666666666</v>
       </c>
       <c r="N44" s="67">
         <f>$F44*Outputs_Internal!K$52/12</f>
-        <v>7307.3362794612794</v>
+        <v>5149.0450336700333</v>
       </c>
       <c r="O44" s="67">
         <f>$F44*Outputs_Internal!L$52/12</f>
-        <v>16318.375</v>
+        <v>6701.708333333333</v>
       </c>
       <c r="P44" s="67">
         <f>$F44*Outputs_Internal!M$52/12</f>
-        <v>1272.2962962962965</v>
+        <v>857.48148148148164</v>
       </c>
       <c r="Q44" s="67">
         <f>$F44*Outputs_Internal!N$52/12</f>
-        <v>131.15909090909091</v>
+        <v>83.431818181818173</v>
       </c>
       <c r="S44" s="67">
         <f>IF(MOD(MONTH($B44),3)=0,SUM(H42:H44,M42:M44),0)</f>
-        <v>58375</v>
+        <v>38375</v>
       </c>
       <c r="T44" s="67">
         <f t="shared" si="2"/>
-        <v>21922.008838383837</v>
+        <v>15447.135101010099</v>
       </c>
       <c r="U44" s="67">
         <f t="shared" si="3"/>
-        <v>48955.125</v>
+        <v>20105.125</v>
       </c>
       <c r="V44" s="67">
         <f t="shared" si="4"/>
-        <v>3816.8888888888896</v>
+        <v>2572.4444444444448</v>
       </c>
       <c r="W44" s="67">
         <f t="shared" si="5"/>
-        <v>393.47727272727275</v>
+        <v>250.2954545454545</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
@@ -11027,11 +11027,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="K93" sqref="K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11231,7 +11231,7 @@
       </c>
       <c r="D9" s="5">
         <f>IF(Inputs!D$4="N",MIN(MAX(Inputs!D$7-$K9,0),$L9-$K9),0)</f>
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="E9" s="5">
         <f>IF(Inputs!E$4="N",MIN(MAX(Inputs!E$7-$K9,0),$L9-$K9),0)</f>
@@ -11266,7 +11266,7 @@
       </c>
       <c r="D10" s="85">
         <f>IFERROR(SUMPRODUCT(D6:D9,$M$6:$M$9)/SUM(D6:D9),0)</f>
-        <v>0.26344827586206898</v>
+        <v>0.40444444444444444</v>
       </c>
       <c r="E10" s="85">
         <f t="shared" ref="E10:H10" si="0">IFERROR(SUMPRODUCT(E6:E9,$M$6:$M$9)/SUM(E6:E9),0)</f>
@@ -11291,7 +11291,7 @@
       </c>
       <c r="D11" s="86">
         <f>SUM(D6:D9)</f>
-        <v>725000</v>
+        <v>225000</v>
       </c>
       <c r="E11" s="86">
         <f t="shared" ref="E11:H11" si="1">SUM(E6:E9)</f>
@@ -11608,7 +11608,7 @@
       </c>
       <c r="D27" s="16">
         <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", "", PRODUCT(D$11, Prices!$E$6)))*D$10</f>
-        <v>76400</v>
+        <v>36400</v>
       </c>
       <c r="E27" s="16">
         <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", "", PRODUCT(E$11, Prices!$E$6)))*E$10</f>
@@ -11653,7 +11653,7 @@
       </c>
       <c r="D29" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D9="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E10),0))*D$10</f>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="E29" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E9="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E10),0))*E$10</f>
@@ -11678,7 +11678,7 @@
       </c>
       <c r="D30" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D10="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E11),0))*D$10</f>
-        <v>13370.000000000002</v>
+        <v>6370.0000000000009</v>
       </c>
       <c r="E30" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E10="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E11),0))*E$10</f>
@@ -11703,7 +11703,7 @@
       </c>
       <c r="D31" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D11="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E12),0))*D$10</f>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="E31" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E11="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E12),0))*E$10</f>
@@ -11728,7 +11728,7 @@
       </c>
       <c r="D32" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D12="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E13),0))*D$10</f>
-        <v>9550</v>
+        <v>4550</v>
       </c>
       <c r="E32" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E12="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E13),0))*E$10</f>
@@ -11753,7 +11753,7 @@
       </c>
       <c r="D33" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D13="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E14),0))*D$10</f>
-        <v>13370.000000000002</v>
+        <v>6370.0000000000009</v>
       </c>
       <c r="E33" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E13="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E14),0))*E$10</f>
@@ -11778,7 +11778,7 @@
       </c>
       <c r="D34" s="18">
         <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D14="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E15),0))*D$10</f>
-        <v>13370.000000000002</v>
+        <v>6370.0000000000009</v>
       </c>
       <c r="E34" s="18">
         <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E14="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E15),0))*E$10</f>
@@ -11802,23 +11802,23 @@
         <v>13</v>
       </c>
       <c r="D35" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
-        <v>47750</v>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D15="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E16),0))*D$10</f>
+        <v>0</v>
       </c>
       <c r="E35" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E15="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E15="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E16),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F35" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F15="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F15="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E16),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G35" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G15="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G15="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E16),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H35" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H15="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H15="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E16),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -11827,23 +11827,23 @@
         <v>14</v>
       </c>
       <c r="D36" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$19="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
-        <v>19100</v>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(OR(Inputs!D16="Y",Inputs!D$20="Y"),PRODUCT(D$11, Prices!$E17),0))*D$10</f>
+        <v>0</v>
       </c>
       <c r="E36" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E16="Y",Inputs!E$19="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(OR(Inputs!E16="Y",Inputs!E$20="Y"),PRODUCT(E$11, Prices!$E17),0))*E$10</f>
         <v>0</v>
       </c>
       <c r="F36" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F16="Y",Inputs!F$19="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(OR(Inputs!F16="Y",Inputs!F$20="Y"),PRODUCT(F$11, Prices!$E17),0))*F$10</f>
         <v>0</v>
       </c>
       <c r="G36" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G16="Y",Inputs!G$19="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(OR(Inputs!G16="Y",Inputs!G$20="Y"),PRODUCT(G$11, Prices!$E17),0))*G$10</f>
         <v>0</v>
       </c>
       <c r="H36" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H16="Y",Inputs!H$19="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(OR(Inputs!H16="Y",Inputs!H$20="Y"),PRODUCT(H$11, Prices!$E17),0))*H$10</f>
         <v>0</v>
       </c>
     </row>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="D53" s="16">
         <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", "", PRODUCT(D$11, Prices!$E$6)*D$10))</f>
-        <v>76400</v>
+        <v>36400</v>
       </c>
       <c r="E53" s="16">
         <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", "", PRODUCT(E$11, Prices!$E$6)*E$10))</f>
@@ -12359,23 +12359,23 @@
         <v>13</v>
       </c>
       <c r="D61" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D15="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E16)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E61" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E15="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E15="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E16)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F61" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F15="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F15="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E16)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G61" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G15="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G15="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E16)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H61" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H15="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H15="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E16)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12384,23 +12384,23 @@
         <v>14</v>
       </c>
       <c r="D62" s="20">
-        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$19="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
+        <f>IF(OR(Inputs!D$4="Y", D$11 = 0), 0, IF(AND(Inputs!D16="Y",Inputs!D$20="N"),PRODUCT(D$11, Prices!$E17)*D$10,0))</f>
         <v>0</v>
       </c>
       <c r="E62" s="20">
-        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E16="Y",Inputs!E$19="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
+        <f>IF(OR(Inputs!E$4="Y", E$11 = 0), 0, IF(AND(Inputs!E16="Y",Inputs!E$20="N"),PRODUCT(E$11, Prices!$E17)*E$10,0))</f>
         <v>0</v>
       </c>
       <c r="F62" s="20">
-        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F16="Y",Inputs!F$19="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
+        <f>IF(OR(Inputs!F$4="Y", F$11 = 0), 0, IF(AND(Inputs!F16="Y",Inputs!F$20="N"),PRODUCT(F$11, Prices!$E17)*F$10,0))</f>
         <v>0</v>
       </c>
       <c r="G62" s="20">
-        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G16="Y",Inputs!G$19="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
+        <f>IF(OR(Inputs!G$4="Y", G$11 = 0), 0, IF(AND(Inputs!G16="Y",Inputs!G$20="N"),PRODUCT(G$11, Prices!$E17)*G$10,0))</f>
         <v>0</v>
       </c>
       <c r="H62" s="20">
-        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H16="Y",Inputs!H$19="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
+        <f>IF(OR(Inputs!H$4="Y", H$11 = 0), 0, IF(AND(Inputs!H16="Y",Inputs!H$20="N"),PRODUCT(H$11, Prices!$E17)*H$10,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -12660,7 +12660,7 @@
       </c>
       <c r="D73" s="18">
         <f>IF(Inputs!D$4="Y", 0, IF(D$11 = "", 0, IF(Inputs!D19 = "Y", D$11*Prices!$E21, 0)))*D$10</f>
-        <v>76400</v>
+        <v>36400</v>
       </c>
       <c r="E73" s="18">
         <f>IF(Inputs!E$4="Y", 0, IF(E$11 = "", 0, IF(Inputs!E19 = "Y", E$11*Prices!$E21, 0)))*E$10</f>
@@ -12892,7 +12892,7 @@
       </c>
       <c r="D85" s="18">
         <f>IF(D73=0,0,D73-SUM(D29:D34))</f>
-        <v>7640</v>
+        <v>3640</v>
       </c>
       <c r="E85" s="18">
         <f t="shared" ref="E85:H85" si="19">IF(E73=0,0,E73-SUM(E29:E34))</f>
@@ -13022,14 +13022,14 @@
       </c>
       <c r="D93" s="7">
         <f>SUM(D40:D50, D53:D63, D66:D69, D72:D75, D90:D91)</f>
-        <v>233500</v>
+        <v>153500</v>
       </c>
       <c r="E93" s="7">
-        <f t="shared" ref="E93:H93" si="22">SUM(E40:E50, E53:E63, E66:E69, E72:E75, E90:E91)</f>
+        <f>SUM(E40:E50, E53:E63, E66:E69, E72:E75, E90:E91)</f>
         <v>0</v>
       </c>
       <c r="F93" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="E93:H93" si="22">SUM(F40:F50, F53:F63, F66:F69, F72:F75, F90:F91)</f>
         <v>0</v>
       </c>
       <c r="G93" s="7">
@@ -13103,7 +13103,7 @@
       </c>
       <c r="D99" s="7">
         <f>SUM(D93, D95)</f>
-        <v>233500</v>
+        <v>153500</v>
       </c>
       <c r="E99" s="7">
         <f>SUM(E93, E95)</f>
@@ -13412,7 +13412,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="39">
-        <f t="shared" ref="F7:H7" si="1">$E7*F$4</f>
+        <f t="shared" ref="F7" si="1">$E7*F$4</f>
         <v>0</v>
       </c>
       <c r="G7" s="39">

</xml_diff>